<commit_message>
Optimizer bug fixed roe data saved
</commit_message>
<xml_diff>
--- a/Rotation/POOL回测表现.xlsx
+++ b/Rotation/POOL回测表现.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\70242\Documents\Python\Ruihui-Intern\Rotation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\meiconte\Documents\RH\Rotation\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{B37B99C2-E456-4026-8B1F-5798DC4869C3}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12135" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12135" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="指数POOL" sheetId="1" r:id="rId1"/>
@@ -17,7 +18,7 @@
     <sheet name="股票POOL" sheetId="2" r:id="rId3"/>
     <sheet name="股票回测报告详细" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -297,7 +298,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="&quot;¥&quot;#,##0.00_);[Red]\(&quot;¥&quot;#,##0.00\)"/>
   </numFmts>
@@ -717,13 +718,43 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -744,56 +775,26 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -833,7 +834,7 @@
         <xdr:cNvPr id="3" name="图片 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4A8F77B7-592C-40C6-A7CE-65FE05D157FE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4A8F77B7-592C-40C6-A7CE-65FE05D157FE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -868,7 +869,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>314326</xdr:colOff>
+      <xdr:colOff>18722</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>32878</xdr:rowOff>
     </xdr:to>
@@ -877,7 +878,7 @@
         <xdr:cNvPr id="4" name="图片 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9B10A7A6-B712-457F-8F78-E0AC03AF1C04}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9B10A7A6-B712-457F-8F78-E0AC03AF1C04}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -912,7 +913,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>293176</xdr:colOff>
+      <xdr:colOff>293175</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
@@ -921,7 +922,7 @@
         <xdr:cNvPr id="5" name="图片 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{AE3F8D54-FEEC-48A0-8455-F57F29C8394A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AE3F8D54-FEEC-48A0-8455-F57F29C8394A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -956,7 +957,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>269508</xdr:colOff>
+      <xdr:colOff>269507</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>9526</xdr:rowOff>
     </xdr:to>
@@ -965,7 +966,7 @@
         <xdr:cNvPr id="6" name="图片 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{5F21DA9A-1B7A-4C6B-9078-7F272CB385AB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5F21DA9A-1B7A-4C6B-9078-7F272CB385AB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1009,7 +1010,7 @@
         <xdr:cNvPr id="7" name="图片 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C4DFD0A1-D23A-41BC-AA21-E44F78A51E2E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C4DFD0A1-D23A-41BC-AA21-E44F78A51E2E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1044,7 +1045,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>342901</xdr:colOff>
+      <xdr:colOff>47297</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>72460</xdr:rowOff>
     </xdr:to>
@@ -1053,7 +1054,7 @@
         <xdr:cNvPr id="9" name="图片 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{8F50C13B-1D38-4F34-9640-F74BD04FE695}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8F50C13B-1D38-4F34-9640-F74BD04FE695}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1088,7 +1089,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>344367</xdr:colOff>
+      <xdr:colOff>344366</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>74375</xdr:rowOff>
     </xdr:to>
@@ -1097,7 +1098,7 @@
         <xdr:cNvPr id="10" name="图片 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{93AC925B-5A90-44DC-A292-EB302144D78B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{93AC925B-5A90-44DC-A292-EB302144D78B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1146,7 +1147,7 @@
         <xdr:cNvPr id="9" name="图片 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{AE466890-A10F-46A2-BB66-6C3692255835}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AE466890-A10F-46A2-BB66-6C3692255835}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1190,7 +1191,7 @@
         <xdr:cNvPr id="10" name="图片 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C7AAA63C-2DAF-44DB-A5E5-9425C0367B19}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C7AAA63C-2DAF-44DB-A5E5-9425C0367B19}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1234,7 +1235,7 @@
         <xdr:cNvPr id="11" name="图片 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{670C713F-0FA1-487E-AFBD-47975E430DEB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{670C713F-0FA1-487E-AFBD-47975E430DEB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1278,7 +1279,7 @@
         <xdr:cNvPr id="12" name="图片 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{BEB444CC-B2FE-42EE-A06F-7ED4D47FFF6E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BEB444CC-B2FE-42EE-A06F-7ED4D47FFF6E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1322,7 +1323,7 @@
         <xdr:cNvPr id="13" name="图片 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A9DAFD42-A61A-453C-ABDB-4DFB36888215}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A9DAFD42-A61A-453C-ABDB-4DFB36888215}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1366,7 +1367,7 @@
         <xdr:cNvPr id="14" name="图片 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{17BB0A07-F028-4998-BC4D-777D06098977}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{17BB0A07-F028-4998-BC4D-777D06098977}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1410,7 +1411,7 @@
         <xdr:cNvPr id="15" name="图片 14">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{FE4F3026-32F5-4061-97E1-641566566DD3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FE4F3026-32F5-4061-97E1-641566566DD3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1454,7 +1455,7 @@
         <xdr:cNvPr id="16" name="图片 15">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A1F7A8F9-639D-486F-92AB-064C832CF0DE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A1F7A8F9-639D-486F-92AB-064C832CF0DE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1779,11 +1780,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:R44"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26:H35"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1795,19 +1796,20 @@
     <col min="6" max="6" width="17.25" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="9" style="1"/>
     <col min="9" max="9" width="15.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:18" ht="23.25" x14ac:dyDescent="0.2">
-      <c r="K1" s="40" t="s">
+      <c r="K1" s="59" t="s">
         <v>23</v>
       </c>
-      <c r="L1" s="41"/>
-      <c r="M1" s="41"/>
-      <c r="N1" s="41"/>
-      <c r="O1" s="41"/>
-      <c r="P1" s="41"/>
-      <c r="Q1" s="41"/>
-      <c r="R1" s="42"/>
+      <c r="L1" s="60"/>
+      <c r="M1" s="60"/>
+      <c r="N1" s="60"/>
+      <c r="O1" s="60"/>
+      <c r="P1" s="60"/>
+      <c r="Q1" s="60"/>
+      <c r="R1" s="61"/>
     </row>
     <row r="2" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B2" s="4" t="s">
@@ -1867,10 +1869,10 @@
       <c r="F3" s="14">
         <v>1.7473000000000001</v>
       </c>
-      <c r="G3" s="43">
-        <v>0</v>
-      </c>
-      <c r="H3" s="46">
+      <c r="G3" s="53">
+        <v>0</v>
+      </c>
+      <c r="H3" s="56">
         <v>0.4</v>
       </c>
       <c r="I3" s="34">
@@ -1902,8 +1904,8 @@
       <c r="F4" s="15">
         <v>1.1667000000000001</v>
       </c>
-      <c r="G4" s="44"/>
-      <c r="H4" s="47"/>
+      <c r="G4" s="54"/>
+      <c r="H4" s="57"/>
       <c r="I4" s="34">
         <v>43336</v>
       </c>
@@ -1933,8 +1935,8 @@
       <c r="F5" s="15">
         <v>1.2677</v>
       </c>
-      <c r="G5" s="44"/>
-      <c r="H5" s="47"/>
+      <c r="G5" s="54"/>
+      <c r="H5" s="57"/>
       <c r="I5" s="34">
         <v>43336</v>
       </c>
@@ -1949,7 +1951,7 @@
       <c r="R5" s="10"/>
     </row>
     <row r="6" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B6" s="49" t="s">
+      <c r="B6" s="62" t="s">
         <v>8</v>
       </c>
       <c r="C6" s="26">
@@ -1964,8 +1966,8 @@
       <c r="F6" s="15">
         <v>1.4861</v>
       </c>
-      <c r="G6" s="45"/>
-      <c r="H6" s="47"/>
+      <c r="G6" s="55"/>
+      <c r="H6" s="57"/>
       <c r="I6" s="34">
         <v>43336</v>
       </c>
@@ -1980,7 +1982,7 @@
       <c r="R6" s="10"/>
     </row>
     <row r="7" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B7" s="50"/>
+      <c r="B7" s="63"/>
       <c r="C7" s="26">
         <v>481000</v>
       </c>
@@ -1996,7 +1998,7 @@
       <c r="G7" s="18">
         <v>-0.3</v>
       </c>
-      <c r="H7" s="47"/>
+      <c r="H7" s="57"/>
       <c r="I7" s="34">
         <v>43336</v>
       </c>
@@ -2011,7 +2013,7 @@
       <c r="R7" s="10"/>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B8" s="51" t="s">
+      <c r="B8" s="52" t="s">
         <v>12</v>
       </c>
       <c r="C8" s="25">
@@ -2026,10 +2028,10 @@
       <c r="F8" s="15">
         <v>0.71309999999999996</v>
       </c>
-      <c r="G8" s="43">
-        <v>0</v>
-      </c>
-      <c r="H8" s="48"/>
+      <c r="G8" s="53">
+        <v>0</v>
+      </c>
+      <c r="H8" s="58"/>
       <c r="I8" s="34">
         <v>43336</v>
       </c>
@@ -2044,7 +2046,7 @@
       <c r="R8" s="10"/>
     </row>
     <row r="9" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B9" s="52"/>
+      <c r="B9" s="64"/>
       <c r="C9" s="25">
         <v>114000</v>
       </c>
@@ -2057,7 +2059,7 @@
       <c r="F9" s="15">
         <v>1.7491000000000001</v>
       </c>
-      <c r="G9" s="44"/>
+      <c r="G9" s="54"/>
       <c r="H9" s="30">
         <v>1</v>
       </c>
@@ -2090,7 +2092,7 @@
       <c r="F10" s="15">
         <v>1.7142999999999999</v>
       </c>
-      <c r="G10" s="44"/>
+      <c r="G10" s="54"/>
       <c r="H10" s="30">
         <v>0.4</v>
       </c>
@@ -2114,7 +2116,7 @@
       <c r="R10" s="10"/>
     </row>
     <row r="11" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B11" s="61" t="e">
+      <c r="B11" s="50" t="e">
         <f>指数POOL!E27:E352010-11-8</f>
         <v>#VALUE!</v>
       </c>
@@ -2130,7 +2132,7 @@
       <c r="F11" s="15">
         <v>1.3587</v>
       </c>
-      <c r="G11" s="44"/>
+      <c r="G11" s="54"/>
       <c r="H11" s="30">
         <v>0.4</v>
       </c>
@@ -2147,7 +2149,7 @@
       <c r="R11" s="10"/>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B12" s="56"/>
+      <c r="B12" s="51"/>
       <c r="C12" s="25">
         <v>240000</v>
       </c>
@@ -2160,7 +2162,7 @@
       <c r="F12" s="15">
         <v>1.6793</v>
       </c>
-      <c r="G12" s="44"/>
+      <c r="G12" s="54"/>
       <c r="H12" s="30">
         <v>0.6</v>
       </c>
@@ -2177,7 +2179,7 @@
       <c r="R12" s="10"/>
     </row>
     <row r="13" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B13" s="56"/>
+      <c r="B13" s="51"/>
       <c r="C13" s="25">
         <v>240000</v>
       </c>
@@ -2190,7 +2192,7 @@
       <c r="F13" s="15">
         <v>2.1916000000000002</v>
       </c>
-      <c r="G13" s="45"/>
+      <c r="G13" s="55"/>
       <c r="H13" s="30">
         <v>0.8</v>
       </c>
@@ -2207,7 +2209,7 @@
       <c r="R13" s="10"/>
     </row>
     <row r="14" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B14" s="56"/>
+      <c r="B14" s="51"/>
       <c r="C14" s="25">
         <v>502000</v>
       </c>
@@ -2220,7 +2222,7 @@
       <c r="F14" s="15">
         <v>1.4412</v>
       </c>
-      <c r="G14" s="53">
+      <c r="G14" s="47">
         <v>-0.3</v>
       </c>
       <c r="H14" s="30">
@@ -2239,7 +2241,7 @@
       <c r="R14" s="10"/>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B15" s="56"/>
+      <c r="B15" s="51"/>
       <c r="C15" s="25">
         <v>502000</v>
       </c>
@@ -2252,7 +2254,7 @@
       <c r="F15" s="15">
         <v>1.7323</v>
       </c>
-      <c r="G15" s="54"/>
+      <c r="G15" s="48"/>
       <c r="H15" s="30">
         <v>0.6</v>
       </c>
@@ -2269,7 +2271,7 @@
       <c r="R15" s="10"/>
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B16" s="56"/>
+      <c r="B16" s="51"/>
       <c r="C16" s="25">
         <v>502000</v>
       </c>
@@ -2282,7 +2284,7 @@
       <c r="F16" s="15">
         <v>2.0663999999999998</v>
       </c>
-      <c r="G16" s="55"/>
+      <c r="G16" s="49"/>
       <c r="H16" s="30">
         <v>0.8</v>
       </c>
@@ -2363,22 +2365,22 @@
       <c r="B27" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="C27" s="63">
+      <c r="C27" s="44">
         <v>77742.399999999994</v>
       </c>
-      <c r="D27" s="63">
+      <c r="D27" s="44">
         <v>203097.79</v>
       </c>
-      <c r="E27" s="63">
+      <c r="E27" s="44">
         <v>-39455.550000000003</v>
       </c>
-      <c r="F27" s="62">
+      <c r="F27" s="43">
         <v>1.6124000000000001</v>
       </c>
-      <c r="G27" s="43">
-        <v>0</v>
-      </c>
-      <c r="H27" s="46">
+      <c r="G27" s="53">
+        <v>0</v>
+      </c>
+      <c r="H27" s="56">
         <v>0.4</v>
       </c>
       <c r="I27" s="34">
@@ -2392,20 +2394,20 @@
       <c r="B28" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="C28" s="63">
+      <c r="C28" s="44">
         <v>30000</v>
       </c>
-      <c r="D28" s="63">
+      <c r="D28" s="44">
         <v>87622.47</v>
       </c>
-      <c r="E28" s="63">
+      <c r="E28" s="44">
         <v>-14621.29</v>
       </c>
-      <c r="F28" s="62">
+      <c r="F28" s="43">
         <v>1.9207000000000001</v>
       </c>
-      <c r="G28" s="44"/>
-      <c r="H28" s="47"/>
+      <c r="G28" s="54"/>
+      <c r="H28" s="57"/>
       <c r="I28" s="34">
         <v>43336</v>
       </c>
@@ -2417,20 +2419,20 @@
       <c r="B29" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="C29" s="63">
+      <c r="C29" s="44">
         <v>63000</v>
       </c>
-      <c r="D29" s="63">
+      <c r="D29" s="44">
         <v>77761.69</v>
       </c>
-      <c r="E29" s="63">
+      <c r="E29" s="44">
         <v>-11683.83</v>
       </c>
-      <c r="F29" s="62">
+      <c r="F29" s="43">
         <v>0.23430000000000001</v>
       </c>
-      <c r="G29" s="44"/>
-      <c r="H29" s="47"/>
+      <c r="G29" s="54"/>
+      <c r="H29" s="57"/>
       <c r="I29" s="34">
         <v>43336</v>
       </c>
@@ -2442,20 +2444,20 @@
       <c r="B30" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="C30" s="63">
+      <c r="C30" s="44">
         <v>15159.57</v>
       </c>
-      <c r="D30" s="63">
+      <c r="D30" s="44">
         <v>34161.71</v>
       </c>
-      <c r="E30" s="63">
+      <c r="E30" s="44">
         <v>-8295.2800000000007</v>
       </c>
-      <c r="F30" s="62">
+      <c r="F30" s="43">
         <v>1.2535000000000001</v>
       </c>
-      <c r="G30" s="44"/>
-      <c r="H30" s="47"/>
+      <c r="G30" s="54"/>
+      <c r="H30" s="57"/>
       <c r="I30" s="34">
         <v>43336</v>
       </c>
@@ -2467,20 +2469,20 @@
       <c r="B31" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="C31" s="63">
+      <c r="C31" s="44">
         <v>65000</v>
       </c>
-      <c r="D31" s="63">
+      <c r="D31" s="44">
         <v>85892.81</v>
       </c>
-      <c r="E31" s="63">
+      <c r="E31" s="44">
         <v>-15026.73</v>
       </c>
-      <c r="F31" s="62">
+      <c r="F31" s="43">
         <v>0.32140000000000002</v>
       </c>
-      <c r="G31" s="44"/>
-      <c r="H31" s="47"/>
+      <c r="G31" s="54"/>
+      <c r="H31" s="57"/>
       <c r="I31" s="34">
         <v>43336</v>
       </c>
@@ -2492,20 +2494,20 @@
       <c r="B32" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="C32" s="63">
+      <c r="C32" s="44">
         <v>69000</v>
       </c>
-      <c r="D32" s="63">
+      <c r="D32" s="44">
         <v>101332.32</v>
       </c>
-      <c r="E32" s="63">
+      <c r="E32" s="44">
         <v>-16532.13</v>
       </c>
-      <c r="F32" s="62">
+      <c r="F32" s="43">
         <v>0.46860000000000002</v>
       </c>
-      <c r="G32" s="44"/>
-      <c r="H32" s="48"/>
+      <c r="G32" s="54"/>
+      <c r="H32" s="58"/>
       <c r="I32" s="34">
         <v>43336</v>
       </c>
@@ -2514,22 +2516,22 @@
       </c>
     </row>
     <row r="33" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B33" s="51" t="s">
+      <c r="B33" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="C33" s="63">
+      <c r="C33" s="44">
         <v>55148.19</v>
       </c>
-      <c r="D33" s="63">
+      <c r="D33" s="44">
         <v>179466.66</v>
       </c>
-      <c r="E33" s="63">
+      <c r="E33" s="44">
         <v>-24719.05</v>
       </c>
-      <c r="F33" s="62">
+      <c r="F33" s="43">
         <v>2.2543000000000002</v>
       </c>
-      <c r="G33" s="44"/>
+      <c r="G33" s="54"/>
       <c r="H33" s="30">
         <v>0.4</v>
       </c>
@@ -2541,20 +2543,20 @@
       </c>
     </row>
     <row r="34" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B34" s="56"/>
-      <c r="C34" s="63">
+      <c r="B34" s="51"/>
+      <c r="C34" s="44">
         <v>127249.3</v>
       </c>
-      <c r="D34" s="63">
+      <c r="D34" s="44">
         <v>271423.44</v>
       </c>
-      <c r="E34" s="63">
+      <c r="E34" s="44">
         <v>-36880.699999999997</v>
       </c>
-      <c r="F34" s="62">
+      <c r="F34" s="43">
         <v>1.133</v>
       </c>
-      <c r="G34" s="44"/>
+      <c r="G34" s="54"/>
       <c r="H34" s="30">
         <v>0.6</v>
       </c>
@@ -2566,20 +2568,20 @@
       </c>
     </row>
     <row r="35" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B35" s="56"/>
-      <c r="C35" s="63">
+      <c r="B35" s="51"/>
+      <c r="C35" s="44">
         <v>124134.55</v>
       </c>
-      <c r="D35" s="63">
+      <c r="D35" s="44">
         <v>303300.68</v>
       </c>
-      <c r="E35" s="63">
+      <c r="E35" s="44">
         <v>-35145.379999999997</v>
       </c>
-      <c r="F35" s="62">
+      <c r="F35" s="43">
         <v>1.4433</v>
       </c>
-      <c r="G35" s="45"/>
+      <c r="G35" s="55"/>
       <c r="H35" s="30">
         <v>0.8</v>
       </c>
@@ -2593,63 +2595,63 @@
     <row r="37" spans="2:13" x14ac:dyDescent="0.2">
       <c r="C37"/>
       <c r="D37"/>
-      <c r="F37" s="59"/>
+      <c r="F37" s="41"/>
     </row>
     <row r="38" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B38" s="64" t="s">
+      <c r="B38" s="45" t="s">
         <v>80</v>
       </c>
       <c r="C38"/>
       <c r="D38"/>
       <c r="E38"/>
-      <c r="F38" s="59"/>
+      <c r="F38" s="41"/>
     </row>
     <row r="39" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B39" s="64" t="s">
+      <c r="B39" s="45" t="s">
         <v>79</v>
       </c>
       <c r="C39"/>
       <c r="D39"/>
-      <c r="F39" s="59"/>
+      <c r="F39" s="41"/>
     </row>
     <row r="40" spans="2:13" x14ac:dyDescent="0.2">
       <c r="C40"/>
       <c r="D40"/>
-      <c r="F40" s="59"/>
+      <c r="F40" s="41"/>
     </row>
     <row r="41" spans="2:13" x14ac:dyDescent="0.2">
       <c r="C41"/>
       <c r="D41"/>
-      <c r="F41" s="59"/>
+      <c r="F41" s="41"/>
     </row>
     <row r="42" spans="2:13" x14ac:dyDescent="0.2">
       <c r="C42"/>
       <c r="D42"/>
-      <c r="F42" s="59"/>
+      <c r="F42" s="41"/>
     </row>
     <row r="43" spans="2:13" x14ac:dyDescent="0.2">
       <c r="C43"/>
       <c r="D43"/>
-      <c r="F43" s="59"/>
+      <c r="F43" s="41"/>
     </row>
     <row r="44" spans="2:13" x14ac:dyDescent="0.2">
       <c r="C44"/>
       <c r="D44"/>
-      <c r="F44" s="59"/>
+      <c r="F44" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="G14:G16"/>
-    <mergeCell ref="B11:B16"/>
-    <mergeCell ref="B33:B35"/>
-    <mergeCell ref="G27:G35"/>
-    <mergeCell ref="H27:H32"/>
     <mergeCell ref="K1:R1"/>
     <mergeCell ref="G3:G6"/>
     <mergeCell ref="H3:H8"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="G8:G13"/>
+    <mergeCell ref="G14:G16"/>
+    <mergeCell ref="B11:B16"/>
+    <mergeCell ref="B33:B35"/>
+    <mergeCell ref="G27:G35"/>
+    <mergeCell ref="H27:H32"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2659,7 +2661,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H304"/>
   <sheetViews>
     <sheetView topLeftCell="A25" workbookViewId="0">
@@ -2698,13 +2700,13 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="58">
+      <c r="A3" s="40">
         <v>39114</v>
       </c>
       <c r="B3" t="s">
         <v>46</v>
       </c>
-      <c r="C3" s="58">
+      <c r="C3" s="40">
         <v>43341</v>
       </c>
     </row>
@@ -2739,7 +2741,7 @@
       <c r="A7" t="s">
         <v>50</v>
       </c>
-      <c r="B7" s="59">
+      <c r="B7" s="41">
         <v>2.2543000000000002</v>
       </c>
     </row>
@@ -2777,19 +2779,19 @@
       <c r="B11" t="s">
         <v>76</v>
       </c>
-      <c r="C11" s="58">
+      <c r="C11" s="40">
         <v>40651</v>
       </c>
-      <c r="D11" s="60">
-        <v>0</v>
-      </c>
-      <c r="E11" s="58" t="s">
-        <v>46</v>
-      </c>
-      <c r="F11" s="58">
+      <c r="D11" s="42">
+        <v>0</v>
+      </c>
+      <c r="E11" s="40" t="s">
+        <v>46</v>
+      </c>
+      <c r="F11" s="40">
         <v>41247</v>
       </c>
-      <c r="G11" s="60">
+      <c r="G11" s="42">
         <v>0</v>
       </c>
     </row>
@@ -2829,19 +2831,19 @@
         <f>-inf%</f>
         <v>#NAME?</v>
       </c>
-      <c r="D14" s="58">
+      <c r="D14" s="40">
         <v>39461</v>
       </c>
-      <c r="E14" s="60">
+      <c r="E14" s="42">
         <v>0</v>
       </c>
       <c r="F14" t="s">
         <v>46</v>
       </c>
-      <c r="G14" s="58">
+      <c r="G14" s="40">
         <v>39595</v>
       </c>
-      <c r="H14" s="60">
+      <c r="H14" s="42">
         <v>0</v>
       </c>
     </row>
@@ -2852,22 +2854,22 @@
       <c r="B15">
         <v>23854.62</v>
       </c>
-      <c r="C15" s="59">
+      <c r="C15" s="41">
         <v>-2.4923000000000002</v>
       </c>
-      <c r="D15" s="58">
+      <c r="D15" s="40">
         <v>39860</v>
       </c>
-      <c r="E15" s="60">
+      <c r="E15" s="42">
         <v>0</v>
       </c>
       <c r="F15" t="s">
         <v>46</v>
       </c>
-      <c r="G15" s="58">
+      <c r="G15" s="40">
         <v>39874</v>
       </c>
-      <c r="H15" s="60">
+      <c r="H15" s="42">
         <v>0</v>
       </c>
     </row>
@@ -2878,22 +2880,22 @@
       <c r="B16">
         <v>723.17</v>
       </c>
-      <c r="C16" s="59">
+      <c r="C16" s="41">
         <v>-0.14369999999999999</v>
       </c>
-      <c r="D16" s="58">
+      <c r="D16" s="40">
         <v>40490</v>
       </c>
-      <c r="E16" s="60">
+      <c r="E16" s="42">
         <v>0</v>
       </c>
       <c r="F16" t="s">
         <v>46</v>
       </c>
-      <c r="G16" s="58">
+      <c r="G16" s="40">
         <v>40543</v>
       </c>
-      <c r="H16" s="60">
+      <c r="H16" s="42">
         <v>0</v>
       </c>
     </row>
@@ -2904,22 +2906,22 @@
       <c r="B17">
         <v>-10317.89</v>
       </c>
-      <c r="C17" s="59">
+      <c r="C17" s="41">
         <v>-0.64549999999999996</v>
       </c>
-      <c r="D17" s="58">
+      <c r="D17" s="40">
         <v>40651</v>
       </c>
-      <c r="E17" s="60">
+      <c r="E17" s="42">
         <v>0</v>
       </c>
       <c r="F17" t="s">
         <v>46</v>
       </c>
-      <c r="G17" s="58">
+      <c r="G17" s="40">
         <v>40905</v>
       </c>
-      <c r="H17" s="60">
+      <c r="H17" s="42">
         <v>0</v>
       </c>
     </row>
@@ -2930,22 +2932,22 @@
       <c r="B18">
         <v>6104.72</v>
       </c>
-      <c r="C18" s="59">
+      <c r="C18" s="41">
         <v>-1.1355</v>
       </c>
-      <c r="D18" s="58">
+      <c r="D18" s="40">
         <v>41036</v>
       </c>
-      <c r="E18" s="60">
+      <c r="E18" s="42">
         <v>0</v>
       </c>
       <c r="F18" t="s">
         <v>46</v>
       </c>
-      <c r="G18" s="58">
+      <c r="G18" s="40">
         <v>41247</v>
       </c>
-      <c r="H18" s="60">
+      <c r="H18" s="42">
         <v>0</v>
       </c>
     </row>
@@ -2956,22 +2958,22 @@
       <c r="B19">
         <v>5329.74</v>
       </c>
-      <c r="C19" s="59">
+      <c r="C19" s="41">
         <v>-0.75580000000000003</v>
       </c>
-      <c r="D19" s="58">
+      <c r="D19" s="40">
         <v>41423</v>
       </c>
-      <c r="E19" s="60">
+      <c r="E19" s="42">
         <v>0</v>
       </c>
       <c r="F19" t="s">
         <v>46</v>
       </c>
-      <c r="G19" s="58">
+      <c r="G19" s="40">
         <v>41453</v>
       </c>
-      <c r="H19" s="60">
+      <c r="H19" s="42">
         <v>0</v>
       </c>
     </row>
@@ -2982,22 +2984,22 @@
       <c r="B20">
         <v>55585.120000000003</v>
       </c>
-      <c r="C20" s="59">
+      <c r="C20" s="41">
         <v>-0.39510000000000001</v>
       </c>
-      <c r="D20" s="58">
+      <c r="D20" s="40">
         <v>41739</v>
       </c>
-      <c r="E20" s="60">
+      <c r="E20" s="42">
         <v>0</v>
       </c>
       <c r="F20" t="s">
         <v>46</v>
       </c>
-      <c r="G20" s="58">
+      <c r="G20" s="40">
         <v>41779</v>
       </c>
-      <c r="H20" s="60">
+      <c r="H20" s="42">
         <v>0</v>
       </c>
     </row>
@@ -3008,22 +3010,22 @@
       <c r="B21">
         <v>2158.86</v>
       </c>
-      <c r="C21" s="59">
+      <c r="C21" s="41">
         <v>-0.02</v>
       </c>
-      <c r="D21" s="58">
+      <c r="D21" s="40">
         <v>42010</v>
       </c>
-      <c r="E21" s="60">
+      <c r="E21" s="42">
         <v>0</v>
       </c>
       <c r="F21" t="s">
         <v>46</v>
       </c>
-      <c r="G21" s="58">
+      <c r="G21" s="40">
         <v>42024</v>
       </c>
-      <c r="H21" s="60">
+      <c r="H21" s="42">
         <v>0</v>
       </c>
     </row>
@@ -3034,22 +3036,22 @@
       <c r="B22">
         <v>1555.9</v>
       </c>
-      <c r="C22" s="59">
+      <c r="C22" s="41">
         <v>-3.2399999999999998E-2</v>
       </c>
-      <c r="D22" s="58">
+      <c r="D22" s="40">
         <v>42703</v>
       </c>
-      <c r="E22" s="60">
+      <c r="E22" s="42">
         <v>0</v>
       </c>
       <c r="F22" t="s">
         <v>46</v>
       </c>
-      <c r="G22" s="58">
+      <c r="G22" s="40">
         <v>42734</v>
       </c>
-      <c r="H22" s="60">
+      <c r="H22" s="42">
         <v>0</v>
       </c>
     </row>
@@ -3060,22 +3062,22 @@
       <c r="B23">
         <v>6924.64</v>
       </c>
-      <c r="C23" s="59">
+      <c r="C23" s="41">
         <v>-3.8300000000000001E-2</v>
       </c>
-      <c r="D23" s="58">
+      <c r="D23" s="40">
         <v>42832</v>
       </c>
-      <c r="E23" s="60">
+      <c r="E23" s="42">
         <v>0</v>
       </c>
       <c r="F23" t="s">
         <v>46</v>
       </c>
-      <c r="G23" s="58">
+      <c r="G23" s="40">
         <v>42867</v>
       </c>
-      <c r="H23" s="60">
+      <c r="H23" s="42">
         <v>0</v>
       </c>
     </row>
@@ -3086,22 +3088,22 @@
       <c r="B24">
         <v>-8498.74</v>
       </c>
-      <c r="C24" s="59">
+      <c r="C24" s="41">
         <v>-0.123</v>
       </c>
-      <c r="D24" s="58">
+      <c r="D24" s="40">
         <v>43171</v>
       </c>
-      <c r="E24" s="60">
+      <c r="E24" s="42">
         <v>0</v>
       </c>
       <c r="F24" t="s">
         <v>46</v>
       </c>
-      <c r="G24" s="58">
+      <c r="G24" s="40">
         <v>43332</v>
       </c>
-      <c r="H24" s="60">
+      <c r="H24" s="42">
         <v>0</v>
       </c>
     </row>
@@ -3136,22 +3138,22 @@
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A28" s="65" t="s">
+      <c r="A28" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="B28" s="65" t="s">
+      <c r="B28" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="C28" s="65" t="s">
+      <c r="C28" s="46" t="s">
         <v>65</v>
       </c>
-      <c r="D28" s="65" t="s">
+      <c r="D28" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="E28" s="65" t="s">
+      <c r="E28" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="F28" s="65" t="s">
+      <c r="F28" s="46" t="s">
         <v>66</v>
       </c>
     </row>
@@ -3213,13 +3215,13 @@
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A37" s="58">
+      <c r="A37" s="40">
         <v>39114</v>
       </c>
       <c r="B37" t="s">
         <v>46</v>
       </c>
-      <c r="C37" s="58">
+      <c r="C37" s="40">
         <v>43341</v>
       </c>
     </row>
@@ -3254,7 +3256,7 @@
       <c r="A41" t="s">
         <v>50</v>
       </c>
-      <c r="B41" s="59">
+      <c r="B41" s="41">
         <v>1.133</v>
       </c>
     </row>
@@ -3292,19 +3294,19 @@
       <c r="B45" t="s">
         <v>77</v>
       </c>
-      <c r="C45" s="58">
+      <c r="C45" s="40">
         <v>40028</v>
       </c>
-      <c r="D45" s="60">
-        <v>0</v>
-      </c>
-      <c r="E45" s="58" t="s">
-        <v>46</v>
-      </c>
-      <c r="F45" s="58">
+      <c r="D45" s="42">
+        <v>0</v>
+      </c>
+      <c r="E45" s="40" t="s">
+        <v>46</v>
+      </c>
+      <c r="F45" s="40">
         <v>41247</v>
       </c>
-      <c r="G45" s="60">
+      <c r="G45" s="42">
         <v>0</v>
       </c>
     </row>
@@ -3344,19 +3346,19 @@
         <f>-inf%</f>
         <v>#NAME?</v>
       </c>
-      <c r="D48" s="58">
+      <c r="D48" s="40">
         <v>39461</v>
       </c>
-      <c r="E48" s="60">
+      <c r="E48" s="42">
         <v>0</v>
       </c>
       <c r="F48" t="s">
         <v>46</v>
       </c>
-      <c r="G48" s="58">
+      <c r="G48" s="40">
         <v>39595</v>
       </c>
-      <c r="H48" s="60">
+      <c r="H48" s="42">
         <v>0</v>
       </c>
     </row>
@@ -3367,22 +3369,22 @@
       <c r="B49">
         <v>27502.78</v>
       </c>
-      <c r="C49" s="59">
+      <c r="C49" s="41">
         <v>-2.4923000000000002</v>
       </c>
-      <c r="D49" s="58">
+      <c r="D49" s="40">
         <v>39860</v>
       </c>
-      <c r="E49" s="60">
+      <c r="E49" s="42">
         <v>0</v>
       </c>
       <c r="F49" t="s">
         <v>46</v>
       </c>
-      <c r="G49" s="58">
+      <c r="G49" s="40">
         <v>39874</v>
       </c>
-      <c r="H49" s="60">
+      <c r="H49" s="42">
         <v>0</v>
       </c>
     </row>
@@ -3393,22 +3395,22 @@
       <c r="B50">
         <v>-6984.35</v>
       </c>
-      <c r="C50" s="59">
+      <c r="C50" s="41">
         <v>-0.47339999999999999</v>
       </c>
-      <c r="D50" s="58">
+      <c r="D50" s="40">
         <v>40183</v>
       </c>
-      <c r="E50" s="60">
+      <c r="E50" s="42">
         <v>0</v>
       </c>
       <c r="F50" t="s">
         <v>46</v>
       </c>
-      <c r="G50" s="58">
+      <c r="G50" s="40">
         <v>40365</v>
       </c>
-      <c r="H50" s="60">
+      <c r="H50" s="42">
         <v>0</v>
       </c>
     </row>
@@ -3419,22 +3421,22 @@
       <c r="B51">
         <v>-16310.08</v>
       </c>
-      <c r="C51" s="59">
+      <c r="C51" s="41">
         <v>-1.1173</v>
       </c>
-      <c r="D51" s="58">
+      <c r="D51" s="40">
         <v>40651</v>
       </c>
-      <c r="E51" s="60">
+      <c r="E51" s="42">
         <v>0</v>
       </c>
       <c r="F51" t="s">
         <v>46</v>
       </c>
-      <c r="G51" s="58">
+      <c r="G51" s="40">
         <v>40905</v>
       </c>
-      <c r="H51" s="60">
+      <c r="H51" s="42">
         <v>0</v>
       </c>
     </row>
@@ -3445,22 +3447,22 @@
       <c r="B52">
         <v>10062.74</v>
       </c>
-      <c r="C52" s="59">
+      <c r="C52" s="41">
         <v>-2.2067999999999999</v>
       </c>
-      <c r="D52" s="58">
+      <c r="D52" s="40">
         <v>41033</v>
       </c>
-      <c r="E52" s="60">
+      <c r="E52" s="42">
         <v>0</v>
       </c>
       <c r="F52" t="s">
         <v>46</v>
       </c>
-      <c r="G52" s="58">
+      <c r="G52" s="40">
         <v>41247</v>
       </c>
-      <c r="H52" s="60">
+      <c r="H52" s="42">
         <v>0</v>
       </c>
     </row>
@@ -3471,22 +3473,22 @@
       <c r="B53">
         <v>-261.98</v>
       </c>
-      <c r="C53" s="59">
+      <c r="C53" s="41">
         <v>-1.2636000000000001</v>
       </c>
-      <c r="D53" s="58">
+      <c r="D53" s="40">
         <v>41311</v>
       </c>
-      <c r="E53" s="60">
+      <c r="E53" s="42">
         <v>0</v>
       </c>
       <c r="F53" t="s">
         <v>46</v>
       </c>
-      <c r="G53" s="58">
+      <c r="G53" s="40">
         <v>41453</v>
       </c>
-      <c r="H53" s="60">
+      <c r="H53" s="42">
         <v>0</v>
       </c>
     </row>
@@ -3497,22 +3499,22 @@
       <c r="B54">
         <v>84825.61</v>
       </c>
-      <c r="C54" s="59">
+      <c r="C54" s="41">
         <v>-1.1697</v>
       </c>
-      <c r="D54" s="58">
+      <c r="D54" s="40">
         <v>41641</v>
       </c>
-      <c r="E54" s="60">
+      <c r="E54" s="42">
         <v>0</v>
       </c>
       <c r="F54" t="s">
         <v>46</v>
       </c>
-      <c r="G54" s="58">
+      <c r="G54" s="40">
         <v>41660</v>
       </c>
-      <c r="H54" s="60">
+      <c r="H54" s="42">
         <v>0</v>
       </c>
     </row>
@@ -3523,22 +3525,22 @@
       <c r="B55">
         <v>20189.98</v>
       </c>
-      <c r="C55" s="59">
+      <c r="C55" s="41">
         <v>-0.21379999999999999</v>
       </c>
-      <c r="D55" s="58">
+      <c r="D55" s="40">
         <v>42009</v>
       </c>
-      <c r="E55" s="60">
+      <c r="E55" s="42">
         <v>0</v>
       </c>
       <c r="F55" t="s">
         <v>46</v>
       </c>
-      <c r="G55" s="58">
+      <c r="G55" s="40">
         <v>42044</v>
       </c>
-      <c r="H55" s="60">
+      <c r="H55" s="42">
         <v>0</v>
       </c>
     </row>
@@ -3549,22 +3551,22 @@
       <c r="B56">
         <v>1555.9</v>
       </c>
-      <c r="C56" s="59">
+      <c r="C56" s="41">
         <v>-2.18E-2</v>
       </c>
-      <c r="D56" s="58">
+      <c r="D56" s="40">
         <v>42703</v>
       </c>
-      <c r="E56" s="60">
+      <c r="E56" s="42">
         <v>0</v>
       </c>
       <c r="F56" t="s">
         <v>46</v>
       </c>
-      <c r="G56" s="58">
+      <c r="G56" s="40">
         <v>42734</v>
       </c>
-      <c r="H56" s="60">
+      <c r="H56" s="42">
         <v>0</v>
       </c>
     </row>
@@ -3575,22 +3577,22 @@
       <c r="B57">
         <v>6961.98</v>
       </c>
-      <c r="C57" s="59">
+      <c r="C57" s="41">
         <v>-2.7400000000000001E-2</v>
       </c>
-      <c r="D57" s="58">
+      <c r="D57" s="40">
         <v>43052</v>
       </c>
-      <c r="E57" s="60">
+      <c r="E57" s="42">
         <v>0</v>
       </c>
       <c r="F57" t="s">
         <v>46</v>
       </c>
-      <c r="G57" s="58">
+      <c r="G57" s="40">
         <v>43077</v>
       </c>
-      <c r="H57" s="60">
+      <c r="H57" s="42">
         <v>0</v>
       </c>
     </row>
@@ -3601,22 +3603,22 @@
       <c r="B58">
         <v>-10819.05</v>
       </c>
-      <c r="C58" s="59">
+      <c r="C58" s="41">
         <v>-0.113</v>
       </c>
-      <c r="D58" s="58">
+      <c r="D58" s="40">
         <v>43124</v>
       </c>
-      <c r="E58" s="60">
+      <c r="E58" s="42">
         <v>0</v>
       </c>
       <c r="F58" t="s">
         <v>46</v>
       </c>
-      <c r="G58" s="58">
+      <c r="G58" s="40">
         <v>43332</v>
       </c>
-      <c r="H58" s="60">
+      <c r="H58" s="42">
         <v>0</v>
       </c>
     </row>
@@ -3651,22 +3653,22 @@
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A62" s="65" t="s">
+      <c r="A62" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="B62" s="65" t="s">
+      <c r="B62" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="C62" s="65" t="s">
+      <c r="C62" s="46" t="s">
         <v>65</v>
       </c>
-      <c r="D62" s="65" t="s">
+      <c r="D62" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="E62" s="65" t="s">
+      <c r="E62" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="F62" s="65" t="s">
+      <c r="F62" s="46" t="s">
         <v>66</v>
       </c>
     </row>
@@ -3728,13 +3730,13 @@
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A71" s="58">
+      <c r="A71" s="40">
         <v>39114</v>
       </c>
       <c r="B71" t="s">
         <v>46</v>
       </c>
-      <c r="C71" s="58">
+      <c r="C71" s="40">
         <v>43341</v>
       </c>
     </row>
@@ -3769,7 +3771,7 @@
       <c r="A75" t="s">
         <v>50</v>
       </c>
-      <c r="B75" s="59">
+      <c r="B75" s="41">
         <v>1.4433</v>
       </c>
     </row>
@@ -3807,19 +3809,19 @@
       <c r="B79" t="s">
         <v>78</v>
       </c>
-      <c r="C79" s="58">
+      <c r="C79" s="40">
         <v>40476</v>
       </c>
-      <c r="D79" s="60">
-        <v>0</v>
-      </c>
-      <c r="E79" s="58" t="s">
-        <v>46</v>
-      </c>
-      <c r="F79" s="58">
+      <c r="D79" s="42">
+        <v>0</v>
+      </c>
+      <c r="E79" s="40" t="s">
+        <v>46</v>
+      </c>
+      <c r="F79" s="40">
         <v>41247</v>
       </c>
-      <c r="G79" s="60">
+      <c r="G79" s="42">
         <v>0</v>
       </c>
     </row>
@@ -3859,19 +3861,19 @@
         <f>-inf%</f>
         <v>#NAME?</v>
       </c>
-      <c r="D82" s="58">
+      <c r="D82" s="40">
         <v>39461</v>
       </c>
-      <c r="E82" s="60">
+      <c r="E82" s="42">
         <v>0</v>
       </c>
       <c r="F82" t="s">
         <v>46</v>
       </c>
-      <c r="G82" s="58">
+      <c r="G82" s="40">
         <v>39595</v>
       </c>
-      <c r="H82" s="60">
+      <c r="H82" s="42">
         <v>0</v>
       </c>
     </row>
@@ -3882,22 +3884,22 @@
       <c r="B83">
         <v>28054.44</v>
       </c>
-      <c r="C83" s="59">
+      <c r="C83" s="41">
         <v>-2.4923000000000002</v>
       </c>
-      <c r="D83" s="58">
+      <c r="D83" s="40">
         <v>39860</v>
       </c>
-      <c r="E83" s="60">
+      <c r="E83" s="42">
         <v>0</v>
       </c>
       <c r="F83" t="s">
         <v>46</v>
       </c>
-      <c r="G83" s="58">
+      <c r="G83" s="40">
         <v>39874</v>
       </c>
-      <c r="H83" s="60">
+      <c r="H83" s="42">
         <v>0</v>
       </c>
     </row>
@@ -3908,22 +3910,22 @@
       <c r="B84">
         <v>-4564</v>
       </c>
-      <c r="C84" s="59">
+      <c r="C84" s="41">
         <v>-0.3584</v>
       </c>
-      <c r="D84" s="58">
+      <c r="D84" s="40">
         <v>40197</v>
       </c>
-      <c r="E84" s="60">
+      <c r="E84" s="42">
         <v>0</v>
       </c>
       <c r="F84" t="s">
         <v>46</v>
       </c>
-      <c r="G84" s="58">
+      <c r="G84" s="40">
         <v>40365</v>
       </c>
-      <c r="H84" s="60">
+      <c r="H84" s="42">
         <v>0</v>
       </c>
     </row>
@@ -3934,22 +3936,22 @@
       <c r="B85">
         <v>-16310.08</v>
       </c>
-      <c r="C85" s="59">
+      <c r="C85" s="41">
         <v>-0.9738</v>
       </c>
-      <c r="D85" s="58">
+      <c r="D85" s="40">
         <v>40651</v>
       </c>
-      <c r="E85" s="60">
+      <c r="E85" s="42">
         <v>0</v>
       </c>
       <c r="F85" t="s">
         <v>46</v>
       </c>
-      <c r="G85" s="58">
+      <c r="G85" s="40">
         <v>40905</v>
       </c>
-      <c r="H85" s="60">
+      <c r="H85" s="42">
         <v>0</v>
       </c>
     </row>
@@ -3960,22 +3962,22 @@
       <c r="B86">
         <v>10062.74</v>
       </c>
-      <c r="C86" s="59">
+      <c r="C86" s="41">
         <v>-1.7304999999999999</v>
       </c>
-      <c r="D86" s="58">
+      <c r="D86" s="40">
         <v>41033</v>
       </c>
-      <c r="E86" s="60">
+      <c r="E86" s="42">
         <v>0</v>
       </c>
       <c r="F86" t="s">
         <v>46</v>
       </c>
-      <c r="G86" s="58">
+      <c r="G86" s="40">
         <v>41247</v>
       </c>
-      <c r="H86" s="60">
+      <c r="H86" s="42">
         <v>0</v>
       </c>
     </row>
@@ -3986,22 +3988,22 @@
       <c r="B87">
         <v>-261.98</v>
       </c>
-      <c r="C87" s="59">
+      <c r="C87" s="41">
         <v>-1.1000000000000001</v>
       </c>
-      <c r="D87" s="58">
+      <c r="D87" s="40">
         <v>41311</v>
       </c>
-      <c r="E87" s="60">
+      <c r="E87" s="42">
         <v>0</v>
       </c>
       <c r="F87" t="s">
         <v>46</v>
       </c>
-      <c r="G87" s="58">
+      <c r="G87" s="40">
         <v>41453</v>
       </c>
-      <c r="H87" s="60">
+      <c r="H87" s="42">
         <v>0</v>
       </c>
     </row>
@@ -4012,22 +4014,22 @@
       <c r="B88">
         <v>83227.899999999994</v>
       </c>
-      <c r="C88" s="59">
+      <c r="C88" s="41">
         <v>-0.90290000000000004</v>
       </c>
-      <c r="D88" s="58">
+      <c r="D88" s="40">
         <v>41687</v>
       </c>
-      <c r="E88" s="60">
+      <c r="E88" s="42">
         <v>0</v>
       </c>
       <c r="F88" t="s">
         <v>46</v>
       </c>
-      <c r="G88" s="58">
+      <c r="G88" s="40">
         <v>41779</v>
       </c>
-      <c r="H88" s="60">
+      <c r="H88" s="42">
         <v>0</v>
       </c>
     </row>
@@ -4038,22 +4040,22 @@
       <c r="B89">
         <v>52987.4</v>
       </c>
-      <c r="C89" s="59">
+      <c r="C89" s="41">
         <v>-0.20349999999999999</v>
       </c>
-      <c r="D89" s="58">
+      <c r="D89" s="40">
         <v>42020</v>
       </c>
-      <c r="E89" s="60">
+      <c r="E89" s="42">
         <v>0</v>
       </c>
       <c r="F89" t="s">
         <v>46</v>
       </c>
-      <c r="G89" s="58">
+      <c r="G89" s="40">
         <v>42044</v>
       </c>
-      <c r="H89" s="60">
+      <c r="H89" s="42">
         <v>0</v>
       </c>
     </row>
@@ -4064,22 +4066,22 @@
       <c r="B90">
         <v>1555.9</v>
       </c>
-      <c r="C90" s="59">
+      <c r="C90" s="41">
         <v>-1.6799999999999999E-2</v>
       </c>
-      <c r="D90" s="58">
+      <c r="D90" s="40">
         <v>42703</v>
       </c>
-      <c r="E90" s="60">
+      <c r="E90" s="42">
         <v>0</v>
       </c>
       <c r="F90" t="s">
         <v>46</v>
       </c>
-      <c r="G90" s="58">
+      <c r="G90" s="40">
         <v>42734</v>
       </c>
-      <c r="H90" s="60">
+      <c r="H90" s="42">
         <v>0</v>
       </c>
     </row>
@@ -4090,22 +4092,22 @@
       <c r="B91">
         <v>6887.04</v>
       </c>
-      <c r="C91" s="59">
+      <c r="C91" s="41">
         <v>-2.3599999999999999E-2</v>
       </c>
-      <c r="D91" s="58">
+      <c r="D91" s="40">
         <v>43052</v>
       </c>
-      <c r="E91" s="60">
+      <c r="E91" s="42">
         <v>0</v>
       </c>
       <c r="F91" t="s">
         <v>46</v>
       </c>
-      <c r="G91" s="58">
+      <c r="G91" s="40">
         <v>43077</v>
       </c>
-      <c r="H91" s="60">
+      <c r="H91" s="42">
         <v>0</v>
       </c>
     </row>
@@ -4116,22 +4118,22 @@
       <c r="B92">
         <v>-11231.83</v>
       </c>
-      <c r="C92" s="59">
+      <c r="C92" s="41">
         <v>-9.3200000000000005E-2</v>
       </c>
-      <c r="D92" s="58">
+      <c r="D92" s="40">
         <v>43124</v>
       </c>
-      <c r="E92" s="60">
+      <c r="E92" s="42">
         <v>0</v>
       </c>
       <c r="F92" t="s">
         <v>46</v>
       </c>
-      <c r="G92" s="58">
+      <c r="G92" s="40">
         <v>43332</v>
       </c>
-      <c r="H92" s="60">
+      <c r="H92" s="42">
         <v>0</v>
       </c>
     </row>
@@ -4166,22 +4168,22 @@
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A96" s="65" t="s">
+      <c r="A96" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="B96" s="65" t="s">
+      <c r="B96" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="C96" s="65" t="s">
+      <c r="C96" s="46" t="s">
         <v>65</v>
       </c>
-      <c r="D96" s="65" t="s">
+      <c r="D96" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="E96" s="65" t="s">
+      <c r="E96" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="F96" s="65" t="s">
+      <c r="F96" s="46" t="s">
         <v>66</v>
       </c>
     </row>
@@ -4243,13 +4245,13 @@
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A105" s="58">
+      <c r="A105" s="40">
         <v>39114</v>
       </c>
       <c r="B105" t="s">
         <v>46</v>
       </c>
-      <c r="C105" s="58">
+      <c r="C105" s="40">
         <v>43341</v>
       </c>
     </row>
@@ -4284,7 +4286,7 @@
       <c r="A109" t="s">
         <v>50</v>
       </c>
-      <c r="B109" s="59">
+      <c r="B109" s="41">
         <v>1.6124000000000001</v>
       </c>
     </row>
@@ -4322,19 +4324,19 @@
       <c r="B113" t="s">
         <v>71</v>
       </c>
-      <c r="C113" s="58">
+      <c r="C113" s="40">
         <v>41311</v>
       </c>
-      <c r="D113" s="60">
+      <c r="D113" s="42">
         <v>0</v>
       </c>
       <c r="E113" t="s">
         <v>46</v>
       </c>
-      <c r="F113" s="58">
+      <c r="F113" s="40">
         <v>41719</v>
       </c>
-      <c r="G113" s="60">
+      <c r="G113" s="42">
         <v>0</v>
       </c>
     </row>
@@ -4370,22 +4372,22 @@
       <c r="B116">
         <v>-5001.21</v>
       </c>
-      <c r="C116" s="59">
+      <c r="C116" s="41">
         <v>-78.115799999999993</v>
       </c>
-      <c r="D116" s="58">
+      <c r="D116" s="40">
         <v>39653</v>
       </c>
-      <c r="E116" s="60">
+      <c r="E116" s="42">
         <v>0</v>
       </c>
       <c r="F116" t="s">
         <v>46</v>
       </c>
-      <c r="G116" s="58">
+      <c r="G116" s="40">
         <v>39749</v>
       </c>
-      <c r="H116" s="60">
+      <c r="H116" s="42">
         <v>0</v>
       </c>
     </row>
@@ -4396,22 +4398,22 @@
       <c r="B117">
         <v>20500.57</v>
       </c>
-      <c r="C117" s="59">
+      <c r="C117" s="41">
         <v>-3.0499000000000001</v>
       </c>
-      <c r="D117" s="58">
+      <c r="D117" s="40">
         <v>39860</v>
       </c>
-      <c r="E117" s="60">
+      <c r="E117" s="42">
         <v>0</v>
       </c>
       <c r="F117" t="s">
         <v>46</v>
       </c>
-      <c r="G117" s="58">
+      <c r="G117" s="40">
         <v>39876</v>
       </c>
-      <c r="H117" s="60">
+      <c r="H117" s="42">
         <v>0</v>
       </c>
     </row>
@@ -4422,22 +4424,22 @@
       <c r="B118">
         <v>723.17</v>
       </c>
-      <c r="C118" s="59">
+      <c r="C118" s="41">
         <v>-0.15620000000000001</v>
       </c>
-      <c r="D118" s="58">
+      <c r="D118" s="40">
         <v>40490</v>
       </c>
-      <c r="E118" s="60">
+      <c r="E118" s="42">
         <v>0</v>
       </c>
       <c r="F118" t="s">
         <v>46</v>
       </c>
-      <c r="G118" s="58">
+      <c r="G118" s="40">
         <v>40543</v>
       </c>
-      <c r="H118" s="60">
+      <c r="H118" s="42">
         <v>0</v>
       </c>
     </row>
@@ -4448,22 +4450,22 @@
       <c r="B119">
         <v>-9365.31</v>
       </c>
-      <c r="C119" s="59">
+      <c r="C119" s="41">
         <v>-0.65229999999999999</v>
       </c>
-      <c r="D119" s="58">
+      <c r="D119" s="40">
         <v>40651</v>
       </c>
-      <c r="E119" s="60">
+      <c r="E119" s="42">
         <v>0</v>
       </c>
       <c r="F119" t="s">
         <v>46</v>
       </c>
-      <c r="G119" s="58">
+      <c r="G119" s="40">
         <v>40905</v>
       </c>
-      <c r="H119" s="60">
+      <c r="H119" s="42">
         <v>0</v>
       </c>
     </row>
@@ -4474,22 +4476,22 @@
       <c r="B120">
         <v>12340.07</v>
       </c>
-      <c r="C120" s="59">
+      <c r="C120" s="41">
         <v>-0.93110000000000004</v>
       </c>
-      <c r="D120" s="58">
+      <c r="D120" s="40">
         <v>41033</v>
       </c>
-      <c r="E120" s="60">
+      <c r="E120" s="42">
         <v>0</v>
       </c>
       <c r="F120" t="s">
         <v>46</v>
       </c>
-      <c r="G120" s="58">
+      <c r="G120" s="40">
         <v>41247</v>
       </c>
-      <c r="H120" s="60">
+      <c r="H120" s="42">
         <v>0</v>
       </c>
     </row>
@@ -4500,22 +4502,22 @@
       <c r="B121">
         <v>-16743.150000000001</v>
       </c>
-      <c r="C121" s="59">
+      <c r="C121" s="41">
         <v>-1.0589999999999999</v>
       </c>
-      <c r="D121" s="58">
+      <c r="D121" s="40">
         <v>41311</v>
       </c>
-      <c r="E121" s="60">
+      <c r="E121" s="42">
         <v>0</v>
       </c>
       <c r="F121" t="s">
         <v>46</v>
       </c>
-      <c r="G121" s="58">
+      <c r="G121" s="40">
         <v>41485</v>
       </c>
-      <c r="H121" s="60">
+      <c r="H121" s="42">
         <v>0</v>
       </c>
     </row>
@@ -4526,22 +4528,22 @@
       <c r="B122">
         <v>69118.490000000005</v>
       </c>
-      <c r="C122" s="59">
+      <c r="C122" s="41">
         <v>-3.6337999999999999</v>
       </c>
-      <c r="D122" s="58">
+      <c r="D122" s="40">
         <v>41641</v>
       </c>
-      <c r="E122" s="60">
+      <c r="E122" s="42">
         <v>0</v>
       </c>
       <c r="F122" t="s">
         <v>46</v>
       </c>
-      <c r="G122" s="58">
+      <c r="G122" s="40">
         <v>41719</v>
       </c>
-      <c r="H122" s="60">
+      <c r="H122" s="42">
         <v>0</v>
       </c>
     </row>
@@ -4552,22 +4554,22 @@
       <c r="B123">
         <v>0</v>
       </c>
-      <c r="C123" s="59">
-        <v>0</v>
-      </c>
-      <c r="D123" s="58">
+      <c r="C123" s="41">
+        <v>0</v>
+      </c>
+      <c r="D123" s="40">
         <v>42009</v>
       </c>
-      <c r="E123" s="60">
+      <c r="E123" s="42">
         <v>0</v>
       </c>
       <c r="F123" t="s">
         <v>46</v>
       </c>
-      <c r="G123" s="58">
+      <c r="G123" s="40">
         <v>42369</v>
       </c>
-      <c r="H123" s="60">
+      <c r="H123" s="42">
         <v>0</v>
       </c>
     </row>
@@ -4578,22 +4580,22 @@
       <c r="B124">
         <v>2574.39</v>
       </c>
-      <c r="C124" s="59">
+      <c r="C124" s="41">
         <v>-3.3700000000000001E-2</v>
       </c>
-      <c r="D124" s="58">
+      <c r="D124" s="40">
         <v>42703</v>
       </c>
-      <c r="E124" s="60">
+      <c r="E124" s="42">
         <v>0</v>
       </c>
       <c r="F124" t="s">
         <v>46</v>
       </c>
-      <c r="G124" s="58">
+      <c r="G124" s="40">
         <v>42734</v>
       </c>
-      <c r="H124" s="60">
+      <c r="H124" s="42">
         <v>0</v>
       </c>
     </row>
@@ -4604,22 +4606,22 @@
       <c r="B125">
         <v>9480.4500000000007</v>
       </c>
-      <c r="C125" s="59">
+      <c r="C125" s="41">
         <v>-1.78E-2</v>
       </c>
-      <c r="D125" s="58">
+      <c r="D125" s="40">
         <v>42948</v>
       </c>
-      <c r="E125" s="60">
+      <c r="E125" s="42">
         <v>0</v>
       </c>
       <c r="F125" t="s">
         <v>46</v>
       </c>
-      <c r="G125" s="58">
+      <c r="G125" s="40">
         <v>42961</v>
       </c>
-      <c r="H125" s="60">
+      <c r="H125" s="42">
         <v>0</v>
       </c>
     </row>
@@ -4630,22 +4632,22 @@
       <c r="B126">
         <v>75.59</v>
       </c>
-      <c r="C126" s="59">
+      <c r="C126" s="41">
         <v>-2.5000000000000001E-3</v>
       </c>
-      <c r="D126" s="58">
+      <c r="D126" s="40">
         <v>43321</v>
       </c>
-      <c r="E126" s="60">
+      <c r="E126" s="42">
         <v>0</v>
       </c>
       <c r="F126" t="s">
         <v>46</v>
       </c>
-      <c r="G126" s="58">
+      <c r="G126" s="40">
         <v>43332</v>
       </c>
-      <c r="H126" s="60">
+      <c r="H126" s="42">
         <v>0</v>
       </c>
     </row>
@@ -4680,7 +4682,7 @@
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A130" s="65" t="s">
+      <c r="A130" s="46" t="s">
         <v>2</v>
       </c>
     </row>
@@ -4742,13 +4744,13 @@
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A139" s="58">
+      <c r="A139" s="40">
         <v>39114</v>
       </c>
       <c r="B139" t="s">
         <v>46</v>
       </c>
-      <c r="C139" s="58">
+      <c r="C139" s="40">
         <v>43341</v>
       </c>
     </row>
@@ -4783,7 +4785,7 @@
       <c r="A143" t="s">
         <v>50</v>
       </c>
-      <c r="B143" s="59">
+      <c r="B143" s="41">
         <v>1.9207000000000001</v>
       </c>
     </row>
@@ -4821,19 +4823,19 @@
       <c r="B147" t="s">
         <v>70</v>
       </c>
-      <c r="C147" s="58">
+      <c r="C147" s="40">
         <v>40981</v>
       </c>
-      <c r="D147" s="60">
+      <c r="D147" s="42">
         <v>0</v>
       </c>
       <c r="E147" t="s">
         <v>46</v>
       </c>
-      <c r="F147" s="58">
+      <c r="F147" s="40">
         <v>41247</v>
       </c>
-      <c r="G147" s="60">
+      <c r="G147" s="42">
         <v>0</v>
       </c>
     </row>
@@ -4873,19 +4875,19 @@
         <f>-inf%</f>
         <v>#NAME?</v>
       </c>
-      <c r="D150" s="58">
+      <c r="D150" s="40">
         <v>39461</v>
       </c>
-      <c r="E150" s="60">
+      <c r="E150" s="42">
         <v>0</v>
       </c>
       <c r="F150" t="s">
         <v>46</v>
       </c>
-      <c r="G150" s="58">
+      <c r="G150" s="40">
         <v>39595</v>
       </c>
-      <c r="H150" s="60">
+      <c r="H150" s="42">
         <v>0</v>
       </c>
     </row>
@@ -4896,22 +4898,22 @@
       <c r="B151">
         <v>17667.55</v>
       </c>
-      <c r="C151" s="59">
+      <c r="C151" s="41">
         <v>-1.4407000000000001</v>
       </c>
-      <c r="D151" s="58">
+      <c r="D151" s="40">
         <v>39867</v>
       </c>
-      <c r="E151" s="60">
+      <c r="E151" s="42">
         <v>0</v>
       </c>
       <c r="F151" t="s">
         <v>46</v>
       </c>
-      <c r="G151" s="58">
+      <c r="G151" s="40">
         <v>39874</v>
       </c>
-      <c r="H151" s="60">
+      <c r="H151" s="42">
         <v>0</v>
       </c>
     </row>
@@ -4922,22 +4924,22 @@
       <c r="B152">
         <v>0</v>
       </c>
-      <c r="C152" s="59">
-        <v>0</v>
-      </c>
-      <c r="D152" s="58">
+      <c r="C152" s="41">
+        <v>0</v>
+      </c>
+      <c r="D152" s="40">
         <v>40182</v>
       </c>
-      <c r="E152" s="60">
+      <c r="E152" s="42">
         <v>0</v>
       </c>
       <c r="F152" t="s">
         <v>46</v>
       </c>
-      <c r="G152" s="58">
+      <c r="G152" s="40">
         <v>40543</v>
       </c>
-      <c r="H152" s="60">
+      <c r="H152" s="42">
         <v>0</v>
       </c>
     </row>
@@ -4948,22 +4950,22 @@
       <c r="B153">
         <v>-2345.63</v>
       </c>
-      <c r="C153" s="59">
+      <c r="C153" s="41">
         <v>-0.2087</v>
       </c>
-      <c r="D153" s="58">
+      <c r="D153" s="40">
         <v>40862</v>
       </c>
-      <c r="E153" s="60">
+      <c r="E153" s="42">
         <v>0</v>
       </c>
       <c r="F153" t="s">
         <v>46</v>
       </c>
-      <c r="G153" s="58">
+      <c r="G153" s="40">
         <v>40907</v>
       </c>
-      <c r="H153" s="60">
+      <c r="H153" s="42">
         <v>0</v>
       </c>
     </row>
@@ -4974,22 +4976,22 @@
       <c r="B154">
         <v>-1104.57</v>
       </c>
-      <c r="C154" s="59">
+      <c r="C154" s="41">
         <v>-0.95779999999999998</v>
       </c>
-      <c r="D154" s="58">
+      <c r="D154" s="40">
         <v>40981</v>
       </c>
-      <c r="E154" s="60">
+      <c r="E154" s="42">
         <v>0</v>
       </c>
       <c r="F154" t="s">
         <v>46</v>
       </c>
-      <c r="G154" s="58">
+      <c r="G154" s="40">
         <v>41247</v>
       </c>
-      <c r="H154" s="60">
+      <c r="H154" s="42">
         <v>0</v>
       </c>
     </row>
@@ -5000,22 +5002,22 @@
       <c r="B155">
         <v>11346.87</v>
       </c>
-      <c r="C155" s="59">
+      <c r="C155" s="41">
         <v>-0.59689999999999999</v>
       </c>
-      <c r="D155" s="58">
+      <c r="D155" s="40">
         <v>41424</v>
       </c>
-      <c r="E155" s="60">
+      <c r="E155" s="42">
         <v>0</v>
       </c>
       <c r="F155" t="s">
         <v>46</v>
       </c>
-      <c r="G155" s="58">
+      <c r="G155" s="40">
         <v>41451</v>
       </c>
-      <c r="H155" s="60">
+      <c r="H155" s="42">
         <v>0</v>
       </c>
     </row>
@@ -5026,22 +5028,22 @@
       <c r="B156">
         <v>18325.580000000002</v>
       </c>
-      <c r="C156" s="59">
+      <c r="C156" s="41">
         <v>-0.29870000000000002</v>
       </c>
-      <c r="D156" s="58">
+      <c r="D156" s="40">
         <v>41687</v>
       </c>
-      <c r="E156" s="60">
+      <c r="E156" s="42">
         <v>0</v>
       </c>
       <c r="F156" t="s">
         <v>46</v>
       </c>
-      <c r="G156" s="58">
+      <c r="G156" s="40">
         <v>41758</v>
       </c>
-      <c r="H156" s="60">
+      <c r="H156" s="42">
         <v>0</v>
       </c>
     </row>
@@ -5052,22 +5054,22 @@
       <c r="B157">
         <v>0</v>
       </c>
-      <c r="C157" s="59">
-        <v>0</v>
-      </c>
-      <c r="D157" s="58">
+      <c r="C157" s="41">
+        <v>0</v>
+      </c>
+      <c r="D157" s="40">
         <v>42009</v>
       </c>
-      <c r="E157" s="60">
+      <c r="E157" s="42">
         <v>0</v>
       </c>
       <c r="F157" t="s">
         <v>46</v>
       </c>
-      <c r="G157" s="58">
+      <c r="G157" s="40">
         <v>42369</v>
       </c>
-      <c r="H157" s="60">
+      <c r="H157" s="42">
         <v>0</v>
       </c>
     </row>
@@ -5078,22 +5080,22 @@
       <c r="B158">
         <v>430.5</v>
       </c>
-      <c r="C158" s="59">
+      <c r="C158" s="41">
         <v>-4.5499999999999999E-2</v>
       </c>
-      <c r="D158" s="58">
+      <c r="D158" s="40">
         <v>42702</v>
       </c>
-      <c r="E158" s="60">
+      <c r="E158" s="42">
         <v>0</v>
       </c>
       <c r="F158" t="s">
         <v>46</v>
       </c>
-      <c r="G158" s="58">
+      <c r="G158" s="40">
         <v>42719</v>
       </c>
-      <c r="H158" s="60">
+      <c r="H158" s="42">
         <v>0</v>
       </c>
     </row>
@@ -5104,22 +5106,22 @@
       <c r="B159">
         <v>-357.5</v>
       </c>
-      <c r="C159" s="59">
+      <c r="C159" s="41">
         <v>-0.1164</v>
       </c>
-      <c r="D159" s="58">
+      <c r="D159" s="40">
         <v>42836</v>
       </c>
-      <c r="E159" s="60">
+      <c r="E159" s="42">
         <v>0</v>
       </c>
       <c r="F159" t="s">
         <v>46</v>
       </c>
-      <c r="G159" s="58">
+      <c r="G159" s="40">
         <v>42888</v>
       </c>
-      <c r="H159" s="60">
+      <c r="H159" s="42">
         <v>0</v>
       </c>
     </row>
@@ -5130,22 +5132,22 @@
       <c r="B160">
         <v>-10168.44</v>
       </c>
-      <c r="C160" s="59">
+      <c r="C160" s="41">
         <v>-0.2762</v>
       </c>
-      <c r="D160" s="58">
+      <c r="D160" s="40">
         <v>43108</v>
       </c>
-      <c r="E160" s="60">
+      <c r="E160" s="42">
         <v>0</v>
       </c>
       <c r="F160" t="s">
         <v>46</v>
       </c>
-      <c r="G160" s="58">
+      <c r="G160" s="40">
         <v>43332</v>
       </c>
-      <c r="H160" s="60">
+      <c r="H160" s="42">
         <v>0</v>
       </c>
     </row>
@@ -5180,7 +5182,7 @@
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A164" s="65" t="s">
+      <c r="A164" s="46" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5242,13 +5244,13 @@
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A173" s="58">
+      <c r="A173" s="40">
         <v>39114</v>
       </c>
       <c r="B173" t="s">
         <v>46</v>
       </c>
-      <c r="C173" s="58">
+      <c r="C173" s="40">
         <v>43341</v>
       </c>
     </row>
@@ -5283,7 +5285,7 @@
       <c r="A177" t="s">
         <v>50</v>
       </c>
-      <c r="B177" s="59">
+      <c r="B177" s="41">
         <v>0.23430000000000001</v>
       </c>
     </row>
@@ -5321,19 +5323,19 @@
       <c r="B181" t="s">
         <v>72</v>
       </c>
-      <c r="C181" s="58">
+      <c r="C181" s="40">
         <v>42836</v>
       </c>
-      <c r="D181" s="60">
+      <c r="D181" s="42">
         <v>0</v>
       </c>
       <c r="E181" t="s">
         <v>46</v>
       </c>
-      <c r="F181" s="58">
+      <c r="F181" s="40">
         <v>43332</v>
       </c>
-      <c r="G181" s="60">
+      <c r="G181" s="42">
         <v>0</v>
       </c>
     </row>
@@ -5369,22 +5371,22 @@
       <c r="B184">
         <v>0</v>
       </c>
-      <c r="C184" s="59">
-        <v>0</v>
-      </c>
-      <c r="D184" s="58">
+      <c r="C184" s="41">
+        <v>0</v>
+      </c>
+      <c r="D184" s="40">
         <v>39461</v>
       </c>
-      <c r="E184" s="60">
+      <c r="E184" s="42">
         <v>0</v>
       </c>
       <c r="F184" t="s">
         <v>46</v>
       </c>
-      <c r="G184" s="58">
+      <c r="G184" s="40">
         <v>39813</v>
       </c>
-      <c r="H184" s="60">
+      <c r="H184" s="42">
         <v>0</v>
       </c>
     </row>
@@ -5395,22 +5397,22 @@
       <c r="B185">
         <v>0</v>
       </c>
-      <c r="C185" s="59">
-        <v>0</v>
-      </c>
-      <c r="D185" s="58">
+      <c r="C185" s="41">
+        <v>0</v>
+      </c>
+      <c r="D185" s="40">
         <v>39818</v>
       </c>
-      <c r="E185" s="60">
+      <c r="E185" s="42">
         <v>0</v>
       </c>
       <c r="F185" t="s">
         <v>46</v>
       </c>
-      <c r="G185" s="58">
+      <c r="G185" s="40">
         <v>40178</v>
       </c>
-      <c r="H185" s="60">
+      <c r="H185" s="42">
         <v>0</v>
       </c>
     </row>
@@ -5421,22 +5423,22 @@
       <c r="B186">
         <v>0</v>
       </c>
-      <c r="C186" s="59">
-        <v>0</v>
-      </c>
-      <c r="D186" s="58">
+      <c r="C186" s="41">
+        <v>0</v>
+      </c>
+      <c r="D186" s="40">
         <v>40182</v>
       </c>
-      <c r="E186" s="60">
+      <c r="E186" s="42">
         <v>0</v>
       </c>
       <c r="F186" t="s">
         <v>46</v>
       </c>
-      <c r="G186" s="58">
+      <c r="G186" s="40">
         <v>40543</v>
       </c>
-      <c r="H186" s="60">
+      <c r="H186" s="42">
         <v>0</v>
       </c>
     </row>
@@ -5451,19 +5453,19 @@
         <f>-inf%</f>
         <v>#NAME?</v>
       </c>
-      <c r="D187" s="58">
+      <c r="D187" s="40">
         <v>40547</v>
       </c>
-      <c r="E187" s="60">
+      <c r="E187" s="42">
         <v>0</v>
       </c>
       <c r="F187" t="s">
         <v>46</v>
       </c>
-      <c r="G187" s="58">
+      <c r="G187" s="40">
         <v>40890</v>
       </c>
-      <c r="H187" s="60">
+      <c r="H187" s="42">
         <v>0</v>
       </c>
     </row>
@@ -5474,22 +5476,22 @@
       <c r="B188">
         <v>-1513.56</v>
       </c>
-      <c r="C188" s="59">
+      <c r="C188" s="41">
         <v>-19.423999999999999</v>
       </c>
-      <c r="D188" s="58">
+      <c r="D188" s="40">
         <v>40919</v>
       </c>
-      <c r="E188" s="60">
+      <c r="E188" s="42">
         <v>0</v>
       </c>
       <c r="F188" t="s">
         <v>46</v>
       </c>
-      <c r="G188" s="58">
+      <c r="G188" s="40">
         <v>40925</v>
       </c>
-      <c r="H188" s="60">
+      <c r="H188" s="42">
         <v>0</v>
       </c>
     </row>
@@ -5500,22 +5502,22 @@
       <c r="B189">
         <v>8297.58</v>
       </c>
-      <c r="C189" s="59">
+      <c r="C189" s="41">
         <v>-1.8338000000000001</v>
       </c>
-      <c r="D189" s="58">
+      <c r="D189" s="40">
         <v>41424</v>
       </c>
-      <c r="E189" s="60">
+      <c r="E189" s="42">
         <v>0</v>
       </c>
       <c r="F189" t="s">
         <v>46</v>
       </c>
-      <c r="G189" s="58">
+      <c r="G189" s="40">
         <v>41464</v>
       </c>
-      <c r="H189" s="60">
+      <c r="H189" s="42">
         <v>0</v>
       </c>
     </row>
@@ -5526,22 +5528,22 @@
       <c r="B190">
         <v>16445.330000000002</v>
       </c>
-      <c r="C190" s="59">
+      <c r="C190" s="41">
         <v>-0.72809999999999997</v>
       </c>
-      <c r="D190" s="58">
+      <c r="D190" s="40">
         <v>41641</v>
       </c>
-      <c r="E190" s="60">
+      <c r="E190" s="42">
         <v>0</v>
       </c>
       <c r="F190" t="s">
         <v>46</v>
       </c>
-      <c r="G190" s="58">
+      <c r="G190" s="40">
         <v>41653</v>
       </c>
-      <c r="H190" s="60">
+      <c r="H190" s="42">
         <v>0</v>
       </c>
     </row>
@@ -5552,22 +5554,22 @@
       <c r="B191">
         <v>0</v>
       </c>
-      <c r="C191" s="59">
-        <v>0</v>
-      </c>
-      <c r="D191" s="58">
+      <c r="C191" s="41">
+        <v>0</v>
+      </c>
+      <c r="D191" s="40">
         <v>42009</v>
       </c>
-      <c r="E191" s="60">
+      <c r="E191" s="42">
         <v>0</v>
       </c>
       <c r="F191" t="s">
         <v>46</v>
       </c>
-      <c r="G191" s="58">
+      <c r="G191" s="40">
         <v>42369</v>
       </c>
-      <c r="H191" s="60">
+      <c r="H191" s="42">
         <v>0</v>
       </c>
     </row>
@@ -5578,22 +5580,22 @@
       <c r="B192">
         <v>757.45</v>
       </c>
-      <c r="C192" s="59">
+      <c r="C192" s="41">
         <v>-7.3099999999999998E-2</v>
       </c>
-      <c r="D192" s="58">
+      <c r="D192" s="40">
         <v>42696</v>
       </c>
-      <c r="E192" s="60">
+      <c r="E192" s="42">
         <v>0</v>
       </c>
       <c r="F192" t="s">
         <v>46</v>
       </c>
-      <c r="G192" s="58">
+      <c r="G192" s="40">
         <v>42717</v>
       </c>
-      <c r="H192" s="60">
+      <c r="H192" s="42">
         <v>0</v>
       </c>
     </row>
@@ -5604,22 +5606,22 @@
       <c r="B193">
         <v>-127.44</v>
       </c>
-      <c r="C193" s="59">
+      <c r="C193" s="41">
         <v>-0.19969999999999999</v>
       </c>
-      <c r="D193" s="58">
+      <c r="D193" s="40">
         <v>42836</v>
       </c>
-      <c r="E193" s="60">
+      <c r="E193" s="42">
         <v>0</v>
       </c>
       <c r="F193" t="s">
         <v>46</v>
       </c>
-      <c r="G193" s="58">
+      <c r="G193" s="40">
         <v>42888</v>
       </c>
-      <c r="H193" s="60">
+      <c r="H193" s="42">
         <v>0</v>
       </c>
     </row>
@@ -5630,22 +5632,22 @@
       <c r="B194">
         <v>-9565.23</v>
       </c>
-      <c r="C194" s="59">
+      <c r="C194" s="41">
         <v>-0.43209999999999998</v>
       </c>
-      <c r="D194" s="58">
+      <c r="D194" s="40">
         <v>43108</v>
       </c>
-      <c r="E194" s="60">
+      <c r="E194" s="42">
         <v>0</v>
       </c>
       <c r="F194" t="s">
         <v>46</v>
       </c>
-      <c r="G194" s="58">
+      <c r="G194" s="40">
         <v>43332</v>
       </c>
-      <c r="H194" s="60">
+      <c r="H194" s="42">
         <v>0</v>
       </c>
     </row>
@@ -5680,7 +5682,7 @@
       </c>
     </row>
     <row r="198" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A198" s="65" t="s">
+      <c r="A198" s="46" t="s">
         <v>65</v>
       </c>
     </row>
@@ -5742,13 +5744,13 @@
       </c>
     </row>
     <row r="207" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A207" s="58">
+      <c r="A207" s="40">
         <v>39114</v>
       </c>
       <c r="B207" t="s">
         <v>46</v>
       </c>
-      <c r="C207" s="58">
+      <c r="C207" s="40">
         <v>43341</v>
       </c>
     </row>
@@ -5783,7 +5785,7 @@
       <c r="A211" t="s">
         <v>50</v>
       </c>
-      <c r="B211" s="59">
+      <c r="B211" s="41">
         <v>1.2535000000000001</v>
       </c>
     </row>
@@ -5821,19 +5823,19 @@
       <c r="B215" t="s">
         <v>73</v>
       </c>
-      <c r="C215" s="58">
+      <c r="C215" s="40">
         <v>43248</v>
       </c>
-      <c r="D215" s="60">
+      <c r="D215" s="42">
         <v>0</v>
       </c>
       <c r="E215" t="s">
         <v>46</v>
       </c>
-      <c r="F215" s="58">
+      <c r="F215" s="40">
         <v>43333</v>
       </c>
-      <c r="G215" s="60">
+      <c r="G215" s="42">
         <v>0</v>
       </c>
     </row>
@@ -5869,22 +5871,22 @@
       <c r="B218">
         <v>0</v>
       </c>
-      <c r="C218" s="59">
-        <v>0</v>
-      </c>
-      <c r="D218" s="58">
+      <c r="C218" s="41">
+        <v>0</v>
+      </c>
+      <c r="D218" s="40">
         <v>39461</v>
       </c>
-      <c r="E218" s="60">
+      <c r="E218" s="42">
         <v>0</v>
       </c>
       <c r="F218" t="s">
         <v>46</v>
       </c>
-      <c r="G218" s="58">
+      <c r="G218" s="40">
         <v>39813</v>
       </c>
-      <c r="H218" s="60">
+      <c r="H218" s="42">
         <v>0</v>
       </c>
     </row>
@@ -5895,22 +5897,22 @@
       <c r="B219">
         <v>0</v>
       </c>
-      <c r="C219" s="59">
-        <v>0</v>
-      </c>
-      <c r="D219" s="58">
+      <c r="C219" s="41">
+        <v>0</v>
+      </c>
+      <c r="D219" s="40">
         <v>39818</v>
       </c>
-      <c r="E219" s="60">
+      <c r="E219" s="42">
         <v>0</v>
       </c>
       <c r="F219" t="s">
         <v>46</v>
       </c>
-      <c r="G219" s="58">
+      <c r="G219" s="40">
         <v>40178</v>
       </c>
-      <c r="H219" s="60">
+      <c r="H219" s="42">
         <v>0</v>
       </c>
     </row>
@@ -5921,22 +5923,22 @@
       <c r="B220">
         <v>0</v>
       </c>
-      <c r="C220" s="59">
-        <v>0</v>
-      </c>
-      <c r="D220" s="58">
+      <c r="C220" s="41">
+        <v>0</v>
+      </c>
+      <c r="D220" s="40">
         <v>40182</v>
       </c>
-      <c r="E220" s="60">
+      <c r="E220" s="42">
         <v>0</v>
       </c>
       <c r="F220" t="s">
         <v>46</v>
       </c>
-      <c r="G220" s="58">
+      <c r="G220" s="40">
         <v>40543</v>
       </c>
-      <c r="H220" s="60">
+      <c r="H220" s="42">
         <v>0</v>
       </c>
     </row>
@@ -5947,22 +5949,22 @@
       <c r="B221">
         <v>0</v>
       </c>
-      <c r="C221" s="59">
-        <v>0</v>
-      </c>
-      <c r="D221" s="58">
+      <c r="C221" s="41">
+        <v>0</v>
+      </c>
+      <c r="D221" s="40">
         <v>40547</v>
       </c>
-      <c r="E221" s="60">
+      <c r="E221" s="42">
         <v>0</v>
       </c>
       <c r="F221" t="s">
         <v>46</v>
       </c>
-      <c r="G221" s="58">
+      <c r="G221" s="40">
         <v>40907</v>
       </c>
-      <c r="H221" s="60">
+      <c r="H221" s="42">
         <v>0</v>
       </c>
     </row>
@@ -5973,22 +5975,22 @@
       <c r="B222">
         <v>286.13</v>
       </c>
-      <c r="C222" s="59">
+      <c r="C222" s="41">
         <v>-4.6502999999999997</v>
       </c>
-      <c r="D222" s="58">
+      <c r="D222" s="40">
         <v>41200</v>
       </c>
-      <c r="E222" s="60">
+      <c r="E222" s="42">
         <v>0</v>
       </c>
       <c r="F222" t="s">
         <v>46</v>
       </c>
-      <c r="G222" s="58">
+      <c r="G222" s="40">
         <v>41247</v>
       </c>
-      <c r="H222" s="60">
+      <c r="H222" s="42">
         <v>0</v>
       </c>
     </row>
@@ -5999,22 +6001,22 @@
       <c r="B223">
         <v>4804.6099999999997</v>
       </c>
-      <c r="C223" s="59">
+      <c r="C223" s="41">
         <v>-0.39779999999999999</v>
       </c>
-      <c r="D223" s="58">
+      <c r="D223" s="40">
         <v>41425</v>
       </c>
-      <c r="E223" s="60">
+      <c r="E223" s="42">
         <v>0</v>
       </c>
       <c r="F223" t="s">
         <v>46</v>
       </c>
-      <c r="G223" s="58">
+      <c r="G223" s="40">
         <v>41451</v>
       </c>
-      <c r="H223" s="60">
+      <c r="H223" s="42">
         <v>0</v>
       </c>
     </row>
@@ -6025,22 +6027,22 @@
       <c r="B224">
         <v>0</v>
       </c>
-      <c r="C224" s="59">
-        <v>0</v>
-      </c>
-      <c r="D224" s="58">
+      <c r="C224" s="41">
+        <v>0</v>
+      </c>
+      <c r="D224" s="40">
         <v>41641</v>
       </c>
-      <c r="E224" s="60">
+      <c r="E224" s="42">
         <v>0</v>
       </c>
       <c r="F224" t="s">
         <v>46</v>
       </c>
-      <c r="G224" s="58">
+      <c r="G224" s="40">
         <v>42004</v>
       </c>
-      <c r="H224" s="60">
+      <c r="H224" s="42">
         <v>0</v>
       </c>
     </row>
@@ -6051,22 +6053,22 @@
       <c r="B225">
         <v>0</v>
       </c>
-      <c r="C225" s="59">
-        <v>0</v>
-      </c>
-      <c r="D225" s="58">
+      <c r="C225" s="41">
+        <v>0</v>
+      </c>
+      <c r="D225" s="40">
         <v>42009</v>
       </c>
-      <c r="E225" s="60">
+      <c r="E225" s="42">
         <v>0</v>
       </c>
       <c r="F225" t="s">
         <v>46</v>
       </c>
-      <c r="G225" s="58">
+      <c r="G225" s="40">
         <v>42369</v>
       </c>
-      <c r="H225" s="60">
+      <c r="H225" s="42">
         <v>0</v>
       </c>
     </row>
@@ -6077,22 +6079,22 @@
       <c r="B226">
         <v>599.57000000000005</v>
       </c>
-      <c r="C226" s="59">
+      <c r="C226" s="41">
         <v>-0.23419999999999999</v>
       </c>
-      <c r="D226" s="58">
+      <c r="D226" s="40">
         <v>42696</v>
       </c>
-      <c r="E226" s="60">
+      <c r="E226" s="42">
         <v>0</v>
       </c>
       <c r="F226" t="s">
         <v>46</v>
       </c>
-      <c r="G226" s="58">
+      <c r="G226" s="40">
         <v>42719</v>
       </c>
-      <c r="H226" s="60">
+      <c r="H226" s="42">
         <v>0</v>
       </c>
     </row>
@@ -6103,22 +6105,22 @@
       <c r="B227">
         <v>1672.18</v>
       </c>
-      <c r="C227" s="59">
+      <c r="C227" s="41">
         <v>-0.36020000000000002</v>
       </c>
-      <c r="D227" s="58">
+      <c r="D227" s="40">
         <v>42818</v>
       </c>
-      <c r="E227" s="60">
+      <c r="E227" s="42">
         <v>0</v>
       </c>
       <c r="F227" t="s">
         <v>46</v>
       </c>
-      <c r="G227" s="58">
+      <c r="G227" s="40">
         <v>42943</v>
       </c>
-      <c r="H227" s="60">
+      <c r="H227" s="42">
         <v>0</v>
       </c>
     </row>
@@ -6129,22 +6131,22 @@
       <c r="B228">
         <v>-1428.28</v>
       </c>
-      <c r="C228" s="59">
+      <c r="C228" s="41">
         <v>-0.63139999999999996</v>
       </c>
-      <c r="D228" s="58">
+      <c r="D228" s="40">
         <v>43248</v>
       </c>
-      <c r="E228" s="60">
+      <c r="E228" s="42">
         <v>0</v>
       </c>
       <c r="F228" t="s">
         <v>46</v>
       </c>
-      <c r="G228" s="58">
+      <c r="G228" s="40">
         <v>43333</v>
       </c>
-      <c r="H228" s="60">
+      <c r="H228" s="42">
         <v>0</v>
       </c>
     </row>
@@ -6179,7 +6181,7 @@
       </c>
     </row>
     <row r="232" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A232" s="65" t="s">
+      <c r="A232" s="46" t="s">
         <v>8</v>
       </c>
     </row>
@@ -6241,13 +6243,13 @@
       </c>
     </row>
     <row r="241" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A241" s="58">
+      <c r="A241" s="40">
         <v>39114</v>
       </c>
       <c r="B241" t="s">
         <v>46</v>
       </c>
-      <c r="C241" s="58">
+      <c r="C241" s="40">
         <v>43341</v>
       </c>
     </row>
@@ -6282,7 +6284,7 @@
       <c r="A245" t="s">
         <v>50</v>
       </c>
-      <c r="B245" s="59">
+      <c r="B245" s="41">
         <v>0.32140000000000002</v>
       </c>
     </row>
@@ -6320,19 +6322,19 @@
       <c r="B249" t="s">
         <v>74</v>
       </c>
-      <c r="C249" s="58">
+      <c r="C249" s="40">
         <v>40981</v>
       </c>
-      <c r="D249" s="60">
+      <c r="D249" s="42">
         <v>0</v>
       </c>
       <c r="E249" t="s">
         <v>46</v>
       </c>
-      <c r="F249" s="58">
+      <c r="F249" s="40">
         <v>41247</v>
       </c>
-      <c r="G249" s="60">
+      <c r="G249" s="42">
         <v>0</v>
       </c>
     </row>
@@ -6368,22 +6370,22 @@
       <c r="B252">
         <v>0</v>
       </c>
-      <c r="C252" s="59">
-        <v>0</v>
-      </c>
-      <c r="D252" s="58">
+      <c r="C252" s="41">
+        <v>0</v>
+      </c>
+      <c r="D252" s="40">
         <v>39461</v>
       </c>
-      <c r="E252" s="60">
+      <c r="E252" s="42">
         <v>0</v>
       </c>
       <c r="F252" t="s">
         <v>46</v>
       </c>
-      <c r="G252" s="58">
+      <c r="G252" s="40">
         <v>39813</v>
       </c>
-      <c r="H252" s="60">
+      <c r="H252" s="42">
         <v>0</v>
       </c>
     </row>
@@ -6394,22 +6396,22 @@
       <c r="B253">
         <v>0</v>
       </c>
-      <c r="C253" s="59">
-        <v>0</v>
-      </c>
-      <c r="D253" s="58">
+      <c r="C253" s="41">
+        <v>0</v>
+      </c>
+      <c r="D253" s="40">
         <v>39818</v>
       </c>
-      <c r="E253" s="60">
+      <c r="E253" s="42">
         <v>0</v>
       </c>
       <c r="F253" t="s">
         <v>46</v>
       </c>
-      <c r="G253" s="58">
+      <c r="G253" s="40">
         <v>40178</v>
       </c>
-      <c r="H253" s="60">
+      <c r="H253" s="42">
         <v>0</v>
       </c>
     </row>
@@ -6420,22 +6422,22 @@
       <c r="B254">
         <v>0</v>
       </c>
-      <c r="C254" s="59">
-        <v>0</v>
-      </c>
-      <c r="D254" s="58">
+      <c r="C254" s="41">
+        <v>0</v>
+      </c>
+      <c r="D254" s="40">
         <v>40182</v>
       </c>
-      <c r="E254" s="60">
+      <c r="E254" s="42">
         <v>0</v>
       </c>
       <c r="F254" t="s">
         <v>46</v>
       </c>
-      <c r="G254" s="58">
+      <c r="G254" s="40">
         <v>40543</v>
       </c>
-      <c r="H254" s="60">
+      <c r="H254" s="42">
         <v>0</v>
       </c>
     </row>
@@ -6450,19 +6452,19 @@
         <f>-inf%</f>
         <v>#NAME?</v>
       </c>
-      <c r="D255" s="58">
+      <c r="D255" s="40">
         <v>40547</v>
       </c>
-      <c r="E255" s="60">
+      <c r="E255" s="42">
         <v>0</v>
       </c>
       <c r="F255" t="s">
         <v>46</v>
       </c>
-      <c r="G255" s="58">
+      <c r="G255" s="40">
         <v>40800</v>
       </c>
-      <c r="H255" s="60">
+      <c r="H255" s="42">
         <v>0</v>
       </c>
     </row>
@@ -6473,22 +6475,22 @@
       <c r="B256">
         <v>-2106.39</v>
       </c>
-      <c r="C256" s="59">
+      <c r="C256" s="41">
         <v>-9.3028999999999993</v>
       </c>
-      <c r="D256" s="58">
+      <c r="D256" s="40">
         <v>40981</v>
       </c>
-      <c r="E256" s="60">
+      <c r="E256" s="42">
         <v>0</v>
       </c>
       <c r="F256" t="s">
         <v>46</v>
       </c>
-      <c r="G256" s="58">
+      <c r="G256" s="40">
         <v>41247</v>
       </c>
-      <c r="H256" s="60">
+      <c r="H256" s="42">
         <v>0</v>
       </c>
     </row>
@@ -6499,22 +6501,22 @@
       <c r="B257">
         <v>29498.04</v>
       </c>
-      <c r="C257" s="59">
+      <c r="C257" s="41">
         <v>-0.92300000000000004</v>
       </c>
-      <c r="D257" s="58">
+      <c r="D257" s="40">
         <v>41339</v>
       </c>
-      <c r="E257" s="60">
+      <c r="E257" s="42">
         <v>0</v>
       </c>
       <c r="F257" t="s">
         <v>46</v>
       </c>
-      <c r="G257" s="58">
+      <c r="G257" s="40">
         <v>41380</v>
       </c>
-      <c r="H257" s="60">
+      <c r="H257" s="42">
         <v>0</v>
       </c>
     </row>
@@ -6525,22 +6527,22 @@
       <c r="B258">
         <v>0</v>
       </c>
-      <c r="C258" s="59">
-        <v>0</v>
-      </c>
-      <c r="D258" s="58">
+      <c r="C258" s="41">
+        <v>0</v>
+      </c>
+      <c r="D258" s="40">
         <v>41641</v>
       </c>
-      <c r="E258" s="60">
+      <c r="E258" s="42">
         <v>0</v>
       </c>
       <c r="F258" t="s">
         <v>46</v>
       </c>
-      <c r="G258" s="58">
+      <c r="G258" s="40">
         <v>42004</v>
       </c>
-      <c r="H258" s="60">
+      <c r="H258" s="42">
         <v>0</v>
       </c>
     </row>
@@ -6551,22 +6553,22 @@
       <c r="B259">
         <v>0</v>
       </c>
-      <c r="C259" s="59">
-        <v>0</v>
-      </c>
-      <c r="D259" s="58">
+      <c r="C259" s="41">
+        <v>0</v>
+      </c>
+      <c r="D259" s="40">
         <v>42009</v>
       </c>
-      <c r="E259" s="60">
+      <c r="E259" s="42">
         <v>0</v>
       </c>
       <c r="F259" t="s">
         <v>46</v>
       </c>
-      <c r="G259" s="58">
+      <c r="G259" s="40">
         <v>42369</v>
       </c>
-      <c r="H259" s="60">
+      <c r="H259" s="42">
         <v>0</v>
       </c>
     </row>
@@ -6577,22 +6579,22 @@
       <c r="B260">
         <v>-1619.27</v>
       </c>
-      <c r="C260" s="59">
+      <c r="C260" s="41">
         <v>-0.12470000000000001</v>
       </c>
-      <c r="D260" s="58">
+      <c r="D260" s="40">
         <v>42577</v>
       </c>
-      <c r="E260" s="60">
+      <c r="E260" s="42">
         <v>0</v>
       </c>
       <c r="F260" t="s">
         <v>46</v>
       </c>
-      <c r="G260" s="58">
+      <c r="G260" s="40">
         <v>42734</v>
       </c>
-      <c r="H260" s="60">
+      <c r="H260" s="42">
         <v>0</v>
       </c>
     </row>
@@ -6603,22 +6605,22 @@
       <c r="B261">
         <v>5838.75</v>
       </c>
-      <c r="C261" s="59">
+      <c r="C261" s="41">
         <v>-0.1467</v>
       </c>
-      <c r="D261" s="58">
+      <c r="D261" s="40">
         <v>43052</v>
       </c>
-      <c r="E261" s="60">
+      <c r="E261" s="42">
         <v>0</v>
       </c>
       <c r="F261" t="s">
         <v>46</v>
       </c>
-      <c r="G261" s="58">
+      <c r="G261" s="40">
         <v>43097</v>
       </c>
-      <c r="H261" s="60">
+      <c r="H261" s="42">
         <v>0</v>
       </c>
     </row>
@@ -6629,22 +6631,22 @@
       <c r="B262">
         <v>-7546.61</v>
       </c>
-      <c r="C262" s="59">
+      <c r="C262" s="41">
         <v>-0.36659999999999998</v>
       </c>
-      <c r="D262" s="58">
+      <c r="D262" s="40">
         <v>43171</v>
       </c>
-      <c r="E262" s="60">
+      <c r="E262" s="42">
         <v>0</v>
       </c>
       <c r="F262" t="s">
         <v>46</v>
       </c>
-      <c r="G262" s="58">
+      <c r="G262" s="40">
         <v>43319</v>
       </c>
-      <c r="H262" s="60">
+      <c r="H262" s="42">
         <v>0</v>
       </c>
     </row>
@@ -6679,7 +6681,7 @@
       </c>
     </row>
     <row r="266" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A266" s="65" t="s">
+      <c r="A266" s="46" t="s">
         <v>12</v>
       </c>
     </row>
@@ -6741,13 +6743,13 @@
       </c>
     </row>
     <row r="275" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A275" s="58">
+      <c r="A275" s="40">
         <v>39114</v>
       </c>
       <c r="B275" t="s">
         <v>46</v>
       </c>
-      <c r="C275" s="58">
+      <c r="C275" s="40">
         <v>43341</v>
       </c>
     </row>
@@ -6782,7 +6784,7 @@
       <c r="A279" t="s">
         <v>50</v>
       </c>
-      <c r="B279" s="59">
+      <c r="B279" s="41">
         <v>0.46860000000000002</v>
       </c>
     </row>
@@ -6820,19 +6822,19 @@
       <c r="B283" t="s">
         <v>75</v>
       </c>
-      <c r="C283" s="58">
+      <c r="C283" s="40">
         <v>41568</v>
       </c>
-      <c r="D283" s="60">
+      <c r="D283" s="42">
         <v>0</v>
       </c>
       <c r="E283" t="s">
         <v>46</v>
       </c>
-      <c r="F283" s="58">
+      <c r="F283" s="40">
         <v>41810</v>
       </c>
-      <c r="G283" s="60">
+      <c r="G283" s="42">
         <v>0</v>
       </c>
     </row>
@@ -6868,22 +6870,22 @@
       <c r="B286">
         <v>0</v>
       </c>
-      <c r="C286" s="59">
-        <v>0</v>
-      </c>
-      <c r="D286" s="58">
+      <c r="C286" s="41">
+        <v>0</v>
+      </c>
+      <c r="D286" s="40">
         <v>39461</v>
       </c>
-      <c r="E286" s="60">
+      <c r="E286" s="42">
         <v>0</v>
       </c>
       <c r="F286" t="s">
         <v>46</v>
       </c>
-      <c r="G286" s="58">
+      <c r="G286" s="40">
         <v>39813</v>
       </c>
-      <c r="H286" s="60">
+      <c r="H286" s="42">
         <v>0</v>
       </c>
     </row>
@@ -6894,22 +6896,22 @@
       <c r="B287">
         <v>0</v>
       </c>
-      <c r="C287" s="59">
-        <v>0</v>
-      </c>
-      <c r="D287" s="58">
+      <c r="C287" s="41">
+        <v>0</v>
+      </c>
+      <c r="D287" s="40">
         <v>39818</v>
       </c>
-      <c r="E287" s="60">
+      <c r="E287" s="42">
         <v>0</v>
       </c>
       <c r="F287" t="s">
         <v>46</v>
       </c>
-      <c r="G287" s="58">
+      <c r="G287" s="40">
         <v>40178</v>
       </c>
-      <c r="H287" s="60">
+      <c r="H287" s="42">
         <v>0</v>
       </c>
     </row>
@@ -6920,22 +6922,22 @@
       <c r="B288">
         <v>0</v>
       </c>
-      <c r="C288" s="59">
-        <v>0</v>
-      </c>
-      <c r="D288" s="58">
+      <c r="C288" s="41">
+        <v>0</v>
+      </c>
+      <c r="D288" s="40">
         <v>40182</v>
       </c>
-      <c r="E288" s="60">
+      <c r="E288" s="42">
         <v>0</v>
       </c>
       <c r="F288" t="s">
         <v>46</v>
       </c>
-      <c r="G288" s="58">
+      <c r="G288" s="40">
         <v>40543</v>
       </c>
-      <c r="H288" s="60">
+      <c r="H288" s="42">
         <v>0</v>
       </c>
     </row>
@@ -6950,19 +6952,19 @@
         <f>-inf%</f>
         <v>#NAME?</v>
       </c>
-      <c r="D289" s="58">
+      <c r="D289" s="40">
         <v>40547</v>
       </c>
-      <c r="E289" s="60">
+      <c r="E289" s="42">
         <v>0</v>
       </c>
       <c r="F289" t="s">
         <v>46</v>
       </c>
-      <c r="G289" s="58">
+      <c r="G289" s="40">
         <v>40813</v>
       </c>
-      <c r="H289" s="60">
+      <c r="H289" s="42">
         <v>0</v>
       </c>
     </row>
@@ -6973,22 +6975,22 @@
       <c r="B290">
         <v>664.69</v>
       </c>
-      <c r="C290" s="59">
+      <c r="C290" s="41">
         <v>-3.8380000000000001</v>
       </c>
-      <c r="D290" s="58">
+      <c r="D290" s="40">
         <v>41103</v>
       </c>
-      <c r="E290" s="60">
+      <c r="E290" s="42">
         <v>0</v>
       </c>
       <c r="F290" t="s">
         <v>46</v>
       </c>
-      <c r="G290" s="58">
+      <c r="G290" s="40">
         <v>41247</v>
       </c>
-      <c r="H290" s="60">
+      <c r="H290" s="42">
         <v>0</v>
       </c>
     </row>
@@ -6999,22 +7001,22 @@
       <c r="B291">
         <v>4654.6499999999996</v>
       </c>
-      <c r="C291" s="59">
+      <c r="C291" s="41">
         <v>-2.4352999999999998</v>
       </c>
-      <c r="D291" s="58">
+      <c r="D291" s="40">
         <v>41278</v>
       </c>
-      <c r="E291" s="60">
+      <c r="E291" s="42">
         <v>0</v>
       </c>
       <c r="F291" t="s">
         <v>46</v>
       </c>
-      <c r="G291" s="58">
+      <c r="G291" s="40">
         <v>41639</v>
       </c>
-      <c r="H291" s="60">
+      <c r="H291" s="42">
         <v>0</v>
       </c>
     </row>
@@ -7025,22 +7027,22 @@
       <c r="B292">
         <v>12813.03</v>
       </c>
-      <c r="C292" s="59">
+      <c r="C292" s="41">
         <v>-2.847</v>
       </c>
-      <c r="D292" s="58">
+      <c r="D292" s="40">
         <v>41743</v>
       </c>
-      <c r="E292" s="60">
+      <c r="E292" s="42">
         <v>0</v>
       </c>
       <c r="F292" t="s">
         <v>46</v>
       </c>
-      <c r="G292" s="58">
+      <c r="G292" s="40">
         <v>41810</v>
       </c>
-      <c r="H292" s="60">
+      <c r="H292" s="42">
         <v>0</v>
       </c>
     </row>
@@ -7051,22 +7053,22 @@
       <c r="B293">
         <v>7630.02</v>
       </c>
-      <c r="C293" s="59">
+      <c r="C293" s="41">
         <v>-0.28889999999999999</v>
       </c>
-      <c r="D293" s="58">
+      <c r="D293" s="40">
         <v>42010</v>
       </c>
-      <c r="E293" s="60">
+      <c r="E293" s="42">
         <v>0</v>
       </c>
       <c r="F293" t="s">
         <v>46</v>
       </c>
-      <c r="G293" s="58">
+      <c r="G293" s="40">
         <v>42024</v>
       </c>
-      <c r="H293" s="60">
+      <c r="H293" s="42">
         <v>0</v>
       </c>
     </row>
@@ -7077,22 +7079,22 @@
       <c r="B294">
         <v>1901.16</v>
       </c>
-      <c r="C294" s="59">
+      <c r="C294" s="41">
         <v>-4.2099999999999999E-2</v>
       </c>
-      <c r="D294" s="58">
+      <c r="D294" s="40">
         <v>42597</v>
       </c>
-      <c r="E294" s="60">
+      <c r="E294" s="42">
         <v>0</v>
       </c>
       <c r="F294" t="s">
         <v>46</v>
       </c>
-      <c r="G294" s="58">
+      <c r="G294" s="40">
         <v>42640</v>
       </c>
-      <c r="H294" s="60">
+      <c r="H294" s="42">
         <v>0</v>
       </c>
     </row>
@@ -7103,22 +7105,22 @@
       <c r="B295">
         <v>4864.5600000000004</v>
       </c>
-      <c r="C295" s="59">
+      <c r="C295" s="41">
         <v>-4.36E-2</v>
       </c>
-      <c r="D295" s="58">
+      <c r="D295" s="40">
         <v>42815</v>
       </c>
-      <c r="E295" s="60">
+      <c r="E295" s="42">
         <v>0</v>
       </c>
       <c r="F295" t="s">
         <v>46</v>
       </c>
-      <c r="G295" s="58">
+      <c r="G295" s="40">
         <v>42866</v>
       </c>
-      <c r="H295" s="60">
+      <c r="H295" s="42">
         <v>0</v>
       </c>
     </row>
@@ -7129,22 +7131,22 @@
       <c r="B296">
         <v>0</v>
       </c>
-      <c r="C296" s="59">
-        <v>0</v>
-      </c>
-      <c r="D296" s="58">
+      <c r="C296" s="41">
+        <v>0</v>
+      </c>
+      <c r="D296" s="40">
         <v>43102</v>
       </c>
-      <c r="E296" s="60">
+      <c r="E296" s="42">
         <v>0</v>
       </c>
       <c r="F296" t="s">
         <v>46</v>
       </c>
-      <c r="G296" s="58">
+      <c r="G296" s="40">
         <v>43342</v>
       </c>
-      <c r="H296" s="60">
+      <c r="H296" s="42">
         <v>0</v>
       </c>
     </row>
@@ -7179,7 +7181,7 @@
       </c>
     </row>
     <row r="300" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A300" s="65" t="s">
+      <c r="A300" s="46" t="s">
         <v>66</v>
       </c>
     </row>
@@ -7226,7 +7228,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:R17"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
@@ -7246,16 +7248,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:18" ht="23.25" x14ac:dyDescent="0.2">
-      <c r="K1" s="40" t="s">
+      <c r="K1" s="59" t="s">
         <v>23</v>
       </c>
-      <c r="L1" s="41"/>
-      <c r="M1" s="41"/>
-      <c r="N1" s="41"/>
-      <c r="O1" s="41"/>
-      <c r="P1" s="41"/>
-      <c r="Q1" s="41"/>
-      <c r="R1" s="42"/>
+      <c r="L1" s="60"/>
+      <c r="M1" s="60"/>
+      <c r="N1" s="60"/>
+      <c r="O1" s="60"/>
+      <c r="P1" s="60"/>
+      <c r="Q1" s="60"/>
+      <c r="R1" s="61"/>
     </row>
     <row r="2" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B2" s="4" t="s">
@@ -7321,7 +7323,7 @@
       <c r="H3" s="21">
         <v>0.4</v>
       </c>
-      <c r="I3" s="57">
+      <c r="I3" s="65">
         <v>43336</v>
       </c>
       <c r="K3" s="9"/>
@@ -7351,7 +7353,7 @@
       </c>
       <c r="G4" s="20"/>
       <c r="H4" s="21"/>
-      <c r="I4" s="57"/>
+      <c r="I4" s="65"/>
       <c r="K4" s="9"/>
       <c r="L4" s="5"/>
       <c r="M4" s="5"/>
@@ -7379,7 +7381,7 @@
       </c>
       <c r="G5" s="20"/>
       <c r="H5" s="21"/>
-      <c r="I5" s="57"/>
+      <c r="I5" s="65"/>
       <c r="K5" s="9"/>
       <c r="L5" s="5"/>
       <c r="M5" s="5"/>
@@ -7407,7 +7409,7 @@
       </c>
       <c r="G6" s="20"/>
       <c r="H6" s="21"/>
-      <c r="I6" s="57"/>
+      <c r="I6" s="65"/>
       <c r="K6" s="9"/>
       <c r="L6" s="5"/>
       <c r="M6" s="5"/>
@@ -7435,7 +7437,7 @@
       </c>
       <c r="G7" s="20"/>
       <c r="H7" s="21"/>
-      <c r="I7" s="57"/>
+      <c r="I7" s="65"/>
       <c r="K7" s="9"/>
       <c r="L7" s="5"/>
       <c r="M7" s="5"/>
@@ -7463,7 +7465,7 @@
       </c>
       <c r="G8" s="20"/>
       <c r="H8" s="21"/>
-      <c r="I8" s="57"/>
+      <c r="I8" s="65"/>
       <c r="K8" s="9"/>
       <c r="L8" s="5"/>
       <c r="M8" s="5"/>
@@ -7491,7 +7493,7 @@
       </c>
       <c r="G9" s="20"/>
       <c r="H9" s="21"/>
-      <c r="I9" s="57"/>
+      <c r="I9" s="65"/>
       <c r="K9" s="9"/>
       <c r="L9" s="5"/>
       <c r="M9" s="5"/>
@@ -7519,7 +7521,7 @@
       </c>
       <c r="G10" s="16"/>
       <c r="H10" s="39"/>
-      <c r="I10" s="57"/>
+      <c r="I10" s="65"/>
       <c r="K10" s="1" t="s">
         <v>34</v>
       </c>
@@ -7619,11 +7621,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L29" sqref="L29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -7659,13 +7661,13 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="58">
+      <c r="A3" s="40">
         <v>39114</v>
       </c>
       <c r="B3" t="s">
         <v>46</v>
       </c>
-      <c r="C3" s="58">
+      <c r="C3" s="40">
         <v>43341</v>
       </c>
     </row>
@@ -7700,7 +7702,7 @@
       <c r="A7" t="s">
         <v>50</v>
       </c>
-      <c r="B7" s="59">
+      <c r="B7" s="41">
         <v>3.7650999999999999</v>
       </c>
     </row>
@@ -7738,19 +7740,19 @@
       <c r="B11" t="s">
         <v>81</v>
       </c>
-      <c r="C11" s="58">
+      <c r="C11" s="40">
         <v>41313</v>
       </c>
-      <c r="D11" s="60">
+      <c r="D11" s="42">
         <v>0</v>
       </c>
       <c r="E11" t="s">
         <v>46</v>
       </c>
-      <c r="F11" s="58">
+      <c r="F11" s="40">
         <v>41450</v>
       </c>
-      <c r="G11" s="60">
+      <c r="G11" s="42">
         <v>0</v>
       </c>
     </row>
@@ -7786,22 +7788,22 @@
       <c r="B14">
         <v>-7457.8</v>
       </c>
-      <c r="C14" s="59">
+      <c r="C14" s="41">
         <v>-54.5837</v>
       </c>
-      <c r="D14" s="58">
+      <c r="D14" s="40">
         <v>39573</v>
       </c>
-      <c r="E14" s="60">
+      <c r="E14" s="42">
         <v>0</v>
       </c>
       <c r="F14" t="s">
         <v>46</v>
       </c>
-      <c r="G14" s="58">
+      <c r="G14" s="40">
         <v>39749</v>
       </c>
-      <c r="H14" s="60">
+      <c r="H14" s="42">
         <v>0</v>
       </c>
     </row>
@@ -7812,22 +7814,22 @@
       <c r="B15">
         <v>34898.559999999998</v>
       </c>
-      <c r="C15" s="59">
+      <c r="C15" s="41">
         <v>-1.2062999999999999</v>
       </c>
-      <c r="D15" s="58">
+      <c r="D15" s="40">
         <v>39860</v>
       </c>
-      <c r="E15" s="60">
+      <c r="E15" s="42">
         <v>0</v>
       </c>
       <c r="F15" t="s">
         <v>46</v>
       </c>
-      <c r="G15" s="58">
+      <c r="G15" s="40">
         <v>39874</v>
       </c>
-      <c r="H15" s="60">
+      <c r="H15" s="42">
         <v>0</v>
       </c>
     </row>
@@ -7838,22 +7840,22 @@
       <c r="B16">
         <v>10682.12</v>
       </c>
-      <c r="C16" s="59">
+      <c r="C16" s="41">
         <v>-9.6000000000000002E-2</v>
       </c>
-      <c r="D16" s="58">
+      <c r="D16" s="40">
         <v>40492</v>
       </c>
-      <c r="E16" s="60">
+      <c r="E16" s="42">
         <v>0</v>
       </c>
       <c r="F16" t="s">
         <v>46</v>
       </c>
-      <c r="G16" s="58">
+      <c r="G16" s="40">
         <v>40500</v>
       </c>
-      <c r="H16" s="60">
+      <c r="H16" s="42">
         <v>0</v>
       </c>
     </row>
@@ -7864,22 +7866,22 @@
       <c r="B17">
         <v>380.01</v>
       </c>
-      <c r="C17" s="59">
+      <c r="C17" s="41">
         <v>-0.18360000000000001</v>
       </c>
-      <c r="D17" s="58">
+      <c r="D17" s="40">
         <v>40742</v>
       </c>
-      <c r="E17" s="60">
+      <c r="E17" s="42">
         <v>0</v>
       </c>
       <c r="F17" t="s">
         <v>46</v>
       </c>
-      <c r="G17" s="58">
+      <c r="G17" s="40">
         <v>40906</v>
       </c>
-      <c r="H17" s="60">
+      <c r="H17" s="42">
         <v>0</v>
       </c>
     </row>
@@ -7890,22 +7892,22 @@
       <c r="B18">
         <v>20953.89</v>
       </c>
-      <c r="C18" s="59">
+      <c r="C18" s="41">
         <v>-0.1827</v>
       </c>
-      <c r="D18" s="58">
+      <c r="D18" s="40">
         <v>41036</v>
       </c>
-      <c r="E18" s="60">
+      <c r="E18" s="42">
         <v>0</v>
       </c>
       <c r="F18" t="s">
         <v>46</v>
       </c>
-      <c r="G18" s="58">
+      <c r="G18" s="40">
         <v>41155</v>
       </c>
-      <c r="H18" s="60">
+      <c r="H18" s="42">
         <v>0</v>
       </c>
     </row>
@@ -7916,22 +7918,22 @@
       <c r="B19">
         <v>12180.02</v>
       </c>
-      <c r="C19" s="59">
+      <c r="C19" s="41">
         <v>-0.2006</v>
       </c>
-      <c r="D19" s="58">
+      <c r="D19" s="40">
         <v>41313</v>
       </c>
-      <c r="E19" s="60">
+      <c r="E19" s="42">
         <v>0</v>
       </c>
       <c r="F19" t="s">
         <v>46</v>
       </c>
-      <c r="G19" s="58">
+      <c r="G19" s="40">
         <v>41450</v>
       </c>
-      <c r="H19" s="60">
+      <c r="H19" s="42">
         <v>0</v>
       </c>
     </row>
@@ -7942,22 +7944,22 @@
       <c r="B20">
         <v>45547</v>
       </c>
-      <c r="C20" s="59">
+      <c r="C20" s="41">
         <v>-0.1263</v>
       </c>
-      <c r="D20" s="58">
+      <c r="D20" s="40">
         <v>41740</v>
       </c>
-      <c r="E20" s="60">
+      <c r="E20" s="42">
         <v>0</v>
       </c>
       <c r="F20" t="s">
         <v>46</v>
       </c>
-      <c r="G20" s="58">
+      <c r="G20" s="40">
         <v>41780</v>
       </c>
-      <c r="H20" s="60">
+      <c r="H20" s="42">
         <v>0</v>
       </c>
     </row>
@@ -7968,22 +7970,22 @@
       <c r="B21">
         <v>9063.2000000000007</v>
       </c>
-      <c r="C21" s="59">
+      <c r="C21" s="41">
         <v>-2.12E-2</v>
       </c>
-      <c r="D21" s="58">
+      <c r="D21" s="40">
         <v>42116</v>
       </c>
-      <c r="E21" s="60">
+      <c r="E21" s="42">
         <v>0</v>
       </c>
       <c r="F21" t="s">
         <v>46</v>
       </c>
-      <c r="G21" s="58">
+      <c r="G21" s="40">
         <v>42132</v>
       </c>
-      <c r="H21" s="60">
+      <c r="H21" s="42">
         <v>0</v>
       </c>
     </row>
@@ -7994,22 +7996,22 @@
       <c r="B22">
         <v>12577.41</v>
       </c>
-      <c r="C22" s="59">
+      <c r="C22" s="41">
         <v>-3.4200000000000001E-2</v>
       </c>
-      <c r="D22" s="58">
+      <c r="D22" s="40">
         <v>42375</v>
       </c>
-      <c r="E22" s="60">
+      <c r="E22" s="42">
         <v>0</v>
       </c>
       <c r="F22" t="s">
         <v>46</v>
       </c>
-      <c r="G22" s="58">
+      <c r="G22" s="40">
         <v>42398</v>
       </c>
-      <c r="H22" s="60">
+      <c r="H22" s="42">
         <v>0</v>
       </c>
     </row>
@@ -8020,22 +8022,22 @@
       <c r="B23">
         <v>23561.9</v>
       </c>
-      <c r="C23" s="59">
+      <c r="C23" s="41">
         <v>-3.0599999999999999E-2</v>
       </c>
-      <c r="D23" s="58">
+      <c r="D23" s="40">
         <v>42817</v>
       </c>
-      <c r="E23" s="60">
+      <c r="E23" s="42">
         <v>0</v>
       </c>
       <c r="F23" t="s">
         <v>46</v>
       </c>
-      <c r="G23" s="58">
+      <c r="G23" s="40">
         <v>42865</v>
       </c>
-      <c r="H23" s="60">
+      <c r="H23" s="42">
         <v>0</v>
       </c>
     </row>
@@ -8046,22 +8048,22 @@
       <c r="B24">
         <v>-3733.07</v>
       </c>
-      <c r="C24" s="59">
+      <c r="C24" s="41">
         <v>-3.9199999999999999E-2</v>
       </c>
-      <c r="D24" s="58">
+      <c r="D24" s="40">
         <v>43248</v>
       </c>
-      <c r="E24" s="60">
+      <c r="E24" s="42">
         <v>0</v>
       </c>
       <c r="F24" t="s">
         <v>46</v>
       </c>
-      <c r="G24" s="58">
+      <c r="G24" s="40">
         <v>43339</v>
       </c>
-      <c r="H24" s="60">
+      <c r="H24" s="42">
         <v>0</v>
       </c>
     </row>

</xml_diff>